<commit_message>
test case 001 test_物件管理_駐車場 Signed-off-by: MaHongTao <mht@shequchina.com>
</commit_message>
<xml_diff>
--- a/test_物件管理/待改test/00test_物件管理_駐車場.xlsx
+++ b/test_物件管理/待改test/00test_物件管理_駐車場.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\elwj\git\AP\ap2\areaparking-test\test_物件管理\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\elwj\git\AP\ap2\areaparking-test\test_物件管理\待改test\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="27765" windowHeight="13650" tabRatio="850" firstSheet="7" activeTab="19"/>
+    <workbookView xWindow="1860" yWindow="0" windowWidth="27765" windowHeight="13650" tabRatio="850" firstSheet="3" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="IN_DB_001" sheetId="19" r:id="rId1"/>
@@ -33,12 +33,12 @@
     <sheet name="EXPECT_008" sheetId="21" r:id="rId19"/>
     <sheet name="テストケース" sheetId="3" r:id="rId20"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2961" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2959" uniqueCount="281">
   <si>
     <t>SQL</t>
   </si>
@@ -568,12 +568,6 @@
     <t>2番地</t>
   </si>
   <si>
-    <t>SEARCH</t>
-  </si>
-  <si>
-    <t>right-panel</t>
-  </si>
-  <si>
     <t>項目名</t>
   </si>
   <si>
@@ -581,9 +575,6 @@
   </si>
   <si>
     <t>項目名称</t>
-  </si>
-  <si>
-    <t>WORD</t>
   </si>
   <si>
     <t>searchbar</t>
@@ -908,7 +899,8 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="宋体"/>
-      <charset val="128"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -1354,7 +1346,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1389,7 +1381,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1601,7 +1593,7 @@
   <dimension ref="A3:BV60"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15:XFD20"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
@@ -5319,7 +5311,7 @@
         <v>166</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="12" customHeight="1">
@@ -5327,7 +5319,7 @@
         <v>166</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
     </row>
   </sheetData>
@@ -6012,7 +6004,7 @@
         <v>166</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="12" customHeight="1">
@@ -6020,7 +6012,7 @@
         <v>166</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>227</v>
+        <v>224</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="14.25">
@@ -6028,36 +6020,36 @@
     </row>
     <row r="16" spans="1:5" ht="14.25">
       <c r="A16" s="27" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.25">
       <c r="A17" s="27"/>
       <c r="B17" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="C17" s="28" t="s">
+        <v>177</v>
+      </c>
+      <c r="D17" s="28" t="s">
         <v>178</v>
-      </c>
-      <c r="C17" s="28" t="s">
-        <v>179</v>
-      </c>
-      <c r="D17" s="28" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="14.25">
       <c r="A18" s="27" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B18" s="29" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C18" s="39" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="14.25">
@@ -6065,7 +6057,7 @@
         <v>166</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -6750,7 +6742,7 @@
         <v>166</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="12" customHeight="1">
@@ -6758,7 +6750,7 @@
         <v>166</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>231</v>
+        <v>228</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="14.25">
@@ -6766,36 +6758,36 @@
     </row>
     <row r="16" spans="1:5" ht="14.25">
       <c r="A16" s="27" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="14.25">
       <c r="A17" s="27"/>
       <c r="B17" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="C17" s="28" t="s">
+        <v>177</v>
+      </c>
+      <c r="D17" s="28" t="s">
         <v>178</v>
-      </c>
-      <c r="C17" s="28" t="s">
-        <v>179</v>
-      </c>
-      <c r="D17" s="28" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="14.25">
       <c r="A18" s="27" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B18" s="29" t="s">
-        <v>228</v>
+        <v>225</v>
       </c>
       <c r="C18" s="39" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="14.25">
@@ -6803,7 +6795,7 @@
         <v>166</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -7457,7 +7449,7 @@
         <v>164</v>
       </c>
       <c r="B1" s="38" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="12" customHeight="1">
@@ -7465,7 +7457,7 @@
         <v>166</v>
       </c>
       <c r="B4" s="15" t="s">
-        <v>234</v>
+        <v>231</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="14.25">
@@ -7473,7 +7465,7 @@
         <v>166</v>
       </c>
       <c r="B5" s="15" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
     </row>
     <row r="7" spans="1:5" customFormat="1" ht="13.5">
@@ -8171,8 +8163,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:J12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -8190,182 +8182,182 @@
   <sheetData>
     <row r="4" spans="2:10">
       <c r="B4" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>235</v>
+      </c>
+      <c r="F4" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="G4" s="7" t="s">
         <v>237</v>
       </c>
-      <c r="D4" s="4" t="s">
-        <v>237</v>
-      </c>
-      <c r="E4" s="5" t="s">
+      <c r="H4" s="7" t="s">
+        <v>236</v>
+      </c>
+      <c r="I4" s="8" t="s">
         <v>238</v>
       </c>
-      <c r="F4" s="6" t="s">
+      <c r="J4" s="9" t="s">
         <v>239</v>
-      </c>
-      <c r="G4" s="7" t="s">
-        <v>240</v>
-      </c>
-      <c r="H4" s="7" t="s">
-        <v>239</v>
-      </c>
-      <c r="I4" s="8" t="s">
-        <v>241</v>
-      </c>
-      <c r="J4" s="9" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="5" spans="2:10">
       <c r="B5" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="I5" s="10" t="s">
         <v>244</v>
       </c>
-      <c r="E5" s="1" t="s">
+      <c r="J5" s="10" t="s">
         <v>245</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>246</v>
-      </c>
-      <c r="I5" s="10" t="s">
-        <v>247</v>
-      </c>
-      <c r="J5" s="10" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="6" spans="2:10">
       <c r="B6" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>248</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>249</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>250</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>252</v>
       </c>
       <c r="I6" s="11"/>
       <c r="J6" s="12" t="s">
-        <v>253</v>
+        <v>250</v>
       </c>
     </row>
     <row r="7" spans="2:10">
       <c r="B7" s="1" t="s">
+        <v>251</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>280</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>252</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>254</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>283</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>255</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>256</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>257</v>
       </c>
       <c r="I7" s="11"/>
       <c r="J7" s="12" t="s">
-        <v>258</v>
+        <v>255</v>
       </c>
     </row>
     <row r="8" spans="2:10">
       <c r="B8" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>257</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>259</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>261</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>262</v>
       </c>
       <c r="I8" s="11"/>
       <c r="J8" s="12" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
     </row>
     <row r="9" spans="2:10">
       <c r="B9" s="1" t="s">
+        <v>261</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>264</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>266</v>
-      </c>
-      <c r="F9" s="1" t="s">
-        <v>267</v>
       </c>
       <c r="I9" s="11"/>
       <c r="J9" s="12" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
     </row>
     <row r="10" spans="2:10">
       <c r="B10" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>267</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>268</v>
+      </c>
+      <c r="F10" s="1" t="s">
         <v>269</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>270</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>271</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>272</v>
       </c>
       <c r="I10" s="11"/>
       <c r="J10" s="12" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
     </row>
     <row r="11" spans="2:10">
       <c r="B11" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>272</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>273</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>274</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>275</v>
-      </c>
-      <c r="F11" s="1" t="s">
-        <v>276</v>
       </c>
       <c r="I11" s="11"/>
       <c r="J11" s="12" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
     </row>
     <row r="12" spans="2:10">
       <c r="B12" s="1" t="s">
+        <v>275</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>276</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="I12" s="10" t="s">
         <v>279</v>
       </c>
-      <c r="E12" s="1" t="s">
-        <v>280</v>
-      </c>
-      <c r="F12" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="I12" s="10" t="s">
-        <v>282</v>
-      </c>
       <c r="J12" s="10" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
     </row>
   </sheetData>
@@ -9008,10 +9000,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C50" sqref="C50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" activeCellId="1" sqref="B10 D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
@@ -9055,46 +9047,38 @@
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
     </row>
-    <row r="9" spans="1:5" ht="14.25">
-      <c r="A9" s="27" t="s">
+    <row r="9" spans="1:5" ht="12" customHeight="1">
+      <c r="A9" s="27"/>
+      <c r="B9" s="28" t="s">
         <v>176</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="C9" s="28" t="s">
         <v>177</v>
       </c>
+      <c r="D9" s="28" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="10" spans="1:5" ht="12" customHeight="1">
-      <c r="A10" s="27"/>
-      <c r="B10" s="28" t="s">
-        <v>178</v>
-      </c>
-      <c r="C10" s="28" t="s">
+      <c r="A10" s="27" t="s">
+        <v>185</v>
+      </c>
+      <c r="B10" s="36" t="s">
         <v>179</v>
       </c>
-      <c r="D10" s="28" t="s">
+      <c r="C10" s="30" t="s">
+        <v>171</v>
+      </c>
+      <c r="D10" s="31" t="s">
         <v>180</v>
       </c>
     </row>
-    <row r="11" spans="1:5" ht="12" customHeight="1">
-      <c r="A11" s="27" t="s">
+    <row r="13" spans="1:5" ht="12" customHeight="1">
+      <c r="A13" s="27" t="s">
+        <v>166</v>
+      </c>
+      <c r="B13" s="15" t="s">
         <v>181</v>
-      </c>
-      <c r="B11" s="29" t="s">
-        <v>182</v>
-      </c>
-      <c r="C11" s="30" t="s">
-        <v>171</v>
-      </c>
-      <c r="D11" s="31" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" ht="12" customHeight="1">
-      <c r="A14" s="27" t="s">
-        <v>166</v>
-      </c>
-      <c r="B14" s="15" t="s">
-        <v>184</v>
       </c>
     </row>
   </sheetData>
@@ -10961,7 +10945,7 @@
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C33" sqref="A34 C33"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
@@ -10979,32 +10963,32 @@
         <v>164</v>
       </c>
       <c r="B1" s="38" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="12" customHeight="1">
       <c r="A3" s="27" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="12" customHeight="1">
       <c r="A4" s="27"/>
       <c r="B4" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="C4" s="28" t="s">
+        <v>177</v>
+      </c>
+      <c r="D4" s="28" t="s">
         <v>178</v>
-      </c>
-      <c r="C4" s="28" t="s">
-        <v>179</v>
-      </c>
-      <c r="D4" s="28" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="12" customHeight="1">
       <c r="A5" s="27" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B5" s="29" t="s">
         <v>18</v>
@@ -11013,12 +10997,12 @@
         <v>100001</v>
       </c>
       <c r="D5" s="31" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="12" customHeight="1">
       <c r="A6" s="27" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B6" s="36" t="s">
         <v>19</v>
@@ -11027,24 +11011,24 @@
         <v>91</v>
       </c>
       <c r="D6" s="31" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="12" customHeight="1">
       <c r="A7" s="27" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B7" s="36" t="s">
         <v>20</v>
       </c>
       <c r="C7" s="30"/>
       <c r="D7" s="31" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="12" customHeight="1">
       <c r="A8" s="27" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B8" s="36" t="s">
         <v>81</v>
@@ -11053,12 +11037,12 @@
         <v>103</v>
       </c>
       <c r="D8" s="31" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="12" customHeight="1">
       <c r="A9" s="27" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B9" s="36" t="s">
         <v>21</v>
@@ -11067,12 +11051,12 @@
         <v>92</v>
       </c>
       <c r="D9" s="31" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="12" customHeight="1">
       <c r="A10" s="27" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B10" s="36" t="s">
         <v>23</v>
@@ -11081,12 +11065,12 @@
         <v>93</v>
       </c>
       <c r="D10" s="31" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="12" customHeight="1">
       <c r="A11" s="27" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B11" s="36" t="s">
         <v>25</v>
@@ -11095,12 +11079,12 @@
         <v>94</v>
       </c>
       <c r="D11" s="31" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="12" customHeight="1">
       <c r="A12" s="27" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B12" s="36" t="s">
         <v>26</v>
@@ -11109,12 +11093,12 @@
         <v>95</v>
       </c>
       <c r="D12" s="31" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="12" customHeight="1">
       <c r="A13" s="27" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B13" s="36" t="s">
         <v>27</v>
@@ -11123,26 +11107,26 @@
         <v>96</v>
       </c>
       <c r="D13" s="31" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="14" spans="1:4" ht="12" customHeight="1">
       <c r="A14" s="27" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B14" s="36" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C14" s="30" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D14" s="31" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="12" customHeight="1">
       <c r="A15" s="27" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B15" s="36" t="s">
         <v>80</v>
@@ -11151,12 +11135,12 @@
         <v>1</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="12" customHeight="1">
       <c r="A16" s="27" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B16" s="36" t="s">
         <v>31</v>
@@ -11165,12 +11149,12 @@
         <v>97</v>
       </c>
       <c r="D16" s="31" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="12" customHeight="1">
       <c r="A17" s="27" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B17" s="15" t="s">
         <v>32</v>
@@ -11184,7 +11168,7 @@
         <v>166</v>
       </c>
       <c r="B22" s="15" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
     </row>
   </sheetData>
@@ -11817,7 +11801,7 @@
     </row>
     <row r="9" spans="1:74" s="14" customFormat="1" ht="12">
       <c r="B9" s="33" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C9" s="34" t="s">
         <v>107</v>
@@ -11932,10 +11916,10 @@
         <v>102</v>
       </c>
       <c r="C11" s="23" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D11" s="23" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E11" s="23" t="s">
         <v>88</v>
@@ -11988,10 +11972,10 @@
         <v>99</v>
       </c>
       <c r="C12" s="23" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D12" s="23" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E12" s="23" t="s">
         <v>88</v>
@@ -12044,10 +12028,10 @@
         <v>126</v>
       </c>
       <c r="C13" s="23" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D13" s="23" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E13" s="23" t="s">
         <v>88</v>
@@ -12100,10 +12084,10 @@
         <v>129</v>
       </c>
       <c r="C14" s="23" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D14" s="23" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E14" s="23" t="s">
         <v>88</v>
@@ -12156,10 +12140,10 @@
         <v>132</v>
       </c>
       <c r="C15" s="23" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D15" s="23" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E15" s="23" t="s">
         <v>88</v>
@@ -12212,10 +12196,10 @@
         <v>104</v>
       </c>
       <c r="C16" s="23" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D16" s="23" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E16" s="23" t="s">
         <v>88</v>
@@ -12268,10 +12252,10 @@
         <v>137</v>
       </c>
       <c r="C17" s="23" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D17" s="23" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E17" s="23" t="s">
         <v>88</v>
@@ -12336,7 +12320,7 @@
     </row>
     <row r="21" spans="1:19" s="15" customFormat="1" ht="12">
       <c r="B21" s="33" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="C21" s="34" t="s">
         <v>107</v>
@@ -12381,10 +12365,10 @@
         <v>102</v>
       </c>
       <c r="C23" s="23" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D23" s="23" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E23" s="23" t="s">
         <v>88</v>
@@ -12416,7 +12400,7 @@
     </row>
     <row r="27" spans="1:19" s="15" customFormat="1" ht="12">
       <c r="B27" s="33" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="C27" s="34" t="s">
         <v>107</v>
@@ -12479,10 +12463,10 @@
         <v>102</v>
       </c>
       <c r="C29" s="23" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D29" s="23" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E29" s="23" t="s">
         <v>88</v>
@@ -12491,7 +12475,7 @@
         <v>89</v>
       </c>
       <c r="G29" s="23" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="H29" s="23" t="s">
         <v>100</v>
@@ -12509,10 +12493,10 @@
         <v>99</v>
       </c>
       <c r="C30" s="23" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D30" s="23" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E30" s="23" t="s">
         <v>88</v>
@@ -12521,7 +12505,7 @@
         <v>89</v>
       </c>
       <c r="G30" s="23" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="H30" s="23" t="s">
         <v>100</v>
@@ -12539,10 +12523,10 @@
         <v>126</v>
       </c>
       <c r="C31" s="23" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D31" s="23" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E31" s="23" t="s">
         <v>88</v>
@@ -12551,7 +12535,7 @@
         <v>89</v>
       </c>
       <c r="G31" s="23" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="H31" s="23" t="s">
         <v>100</v>
@@ -12569,10 +12553,10 @@
         <v>129</v>
       </c>
       <c r="C32" s="23" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="D32" s="23" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="E32" s="23" t="s">
         <v>88</v>
@@ -12581,7 +12565,7 @@
         <v>89</v>
       </c>
       <c r="G32" s="23" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="H32" s="23" t="s">
         <v>100</v>
@@ -12599,10 +12583,10 @@
         <v>132</v>
       </c>
       <c r="C33" s="23" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D33" s="23" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E33" s="23" t="s">
         <v>88</v>
@@ -12611,7 +12595,7 @@
         <v>89</v>
       </c>
       <c r="G33" s="23" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="H33" s="23" t="s">
         <v>100</v>
@@ -12629,10 +12613,10 @@
         <v>104</v>
       </c>
       <c r="C34" s="23" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D34" s="23" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E34" s="23" t="s">
         <v>88</v>
@@ -12641,7 +12625,7 @@
         <v>89</v>
       </c>
       <c r="G34" s="23" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="H34" s="23" t="s">
         <v>100</v>
@@ -12659,10 +12643,10 @@
         <v>137</v>
       </c>
       <c r="C35" s="23" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="D35" s="23" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="E35" s="23" t="s">
         <v>88</v>
@@ -12671,7 +12655,7 @@
         <v>89</v>
       </c>
       <c r="G35" s="23" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="H35" s="23" t="s">
         <v>100</v>
@@ -12695,7 +12679,7 @@
     </row>
     <row r="39" spans="1:13" s="14" customFormat="1" ht="12">
       <c r="B39" s="33" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="C39" s="34" t="s">
         <v>107</v>
@@ -12774,10 +12758,10 @@
         <v>102</v>
       </c>
       <c r="C41" s="23" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="D41" s="23" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="E41" s="23" t="s">
         <v>88</v>
@@ -12812,10 +12796,10 @@
         <v>99</v>
       </c>
       <c r="C42" s="23" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="D42" s="23" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="E42" s="23" t="s">
         <v>88</v>
@@ -12850,10 +12834,10 @@
         <v>126</v>
       </c>
       <c r="C43" s="23" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="D43" s="23" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="E43" s="23" t="s">
         <v>88</v>
@@ -12896,7 +12880,7 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="I40" sqref="I40"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
@@ -12945,32 +12929,32 @@
         <v>166</v>
       </c>
       <c r="B9" s="15" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="12" spans="1:5" ht="12" customHeight="1">
       <c r="A12" s="27" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
     </row>
     <row r="13" spans="1:5" ht="12" customHeight="1">
       <c r="A13" s="27"/>
       <c r="B13" s="28" t="s">
+        <v>176</v>
+      </c>
+      <c r="C13" s="28" t="s">
+        <v>177</v>
+      </c>
+      <c r="D13" s="28" t="s">
         <v>178</v>
-      </c>
-      <c r="C13" s="28" t="s">
-        <v>179</v>
-      </c>
-      <c r="D13" s="28" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="14" spans="1:5" ht="12" customHeight="1">
       <c r="A14" s="27" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B14" s="29" t="s">
         <v>18</v>
@@ -12979,52 +12963,52 @@
         <v>100001</v>
       </c>
       <c r="D14" s="31" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="12" customHeight="1">
       <c r="A15" s="27" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B15" s="36" t="s">
         <v>19</v>
       </c>
       <c r="C15" s="30" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="D15" s="31" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="12" customHeight="1">
       <c r="A16" s="27" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B16" s="36" t="s">
         <v>20</v>
       </c>
       <c r="C16" s="30"/>
       <c r="D16" s="31" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="12" customHeight="1">
       <c r="A17" s="27" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B17" s="36" t="s">
         <v>81</v>
       </c>
       <c r="C17" s="30" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="12" customHeight="1">
       <c r="A18" s="27" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B18" s="36" t="s">
         <v>21</v>
@@ -13033,82 +13017,82 @@
         <v>92</v>
       </c>
       <c r="D18" s="31" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="12" customHeight="1">
       <c r="A19" s="27" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B19" s="36" t="s">
         <v>23</v>
       </c>
       <c r="C19" s="30" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D19" s="31" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="12" customHeight="1">
       <c r="A20" s="27" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B20" s="36" t="s">
         <v>25</v>
       </c>
       <c r="C20" s="30" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="D20" s="31" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="12" customHeight="1">
       <c r="A21" s="27" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B21" s="36" t="s">
         <v>26</v>
       </c>
       <c r="C21" s="30" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="D21" s="31" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="12" customHeight="1">
       <c r="A22" s="27" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B22" s="36" t="s">
         <v>27</v>
       </c>
       <c r="C22" s="30" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="D22" s="31" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="12" customHeight="1">
       <c r="A23" s="27" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B23" s="36" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="C23" s="30" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="D23" s="31" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="12" customHeight="1">
       <c r="A24" s="27" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B24" s="36" t="s">
         <v>80</v>
@@ -13117,32 +13101,32 @@
         <v>0</v>
       </c>
       <c r="D24" s="31" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="12" customHeight="1">
       <c r="A25" s="27" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B25" s="36" t="s">
         <v>31</v>
       </c>
       <c r="C25" s="30" t="s">
-        <v>222</v>
+        <v>219</v>
       </c>
       <c r="D25" s="31" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
     </row>
     <row r="26" spans="1:4" ht="12" customHeight="1">
       <c r="A26" s="27" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="B26" s="15" t="s">
         <v>32</v>
       </c>
       <c r="C26" s="15" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
     </row>
     <row r="30" spans="1:4" ht="12" customHeight="1">
@@ -13150,7 +13134,7 @@
         <v>166</v>
       </c>
       <c r="B30" s="15" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="14.25">
@@ -13158,7 +13142,7 @@
         <v>166</v>
       </c>
       <c r="B31" s="15" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
fix test_物件管理_駐車場 add test_ホワイトボート_駐車場 Signed-off-by: MaHongTao <mht@shequchina.com>
</commit_message>
<xml_diff>
--- a/test_物件管理/待改test/00test_物件管理_駐車場.xlsx
+++ b/test_物件管理/待改test/00test_物件管理_駐車場.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Work\elwj\git\AP\ap2\areaparking-test\test_物件管理\待改test\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="1860" yWindow="0" windowWidth="27765" windowHeight="13650" tabRatio="850" firstSheet="3" activeTab="3"/>
+    <workbookView windowWidth="23250" windowHeight="13650" tabRatio="850" firstSheet="3" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="IN_DB_001" sheetId="19" r:id="rId1"/>
@@ -33,12 +28,12 @@
     <sheet name="EXPECT_008" sheetId="21" r:id="rId19"/>
     <sheet name="テストケース" sheetId="3" r:id="rId20"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2959" uniqueCount="281">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281">
   <si>
     <t>SQL</t>
   </si>
@@ -577,6 +572,9 @@
     <t>項目名称</t>
   </si>
   <si>
+    <t>FIELD</t>
+  </si>
+  <si>
     <t>searchbar</t>
   </si>
   <si>
@@ -595,9 +593,6 @@
     <t>parkinglot_form</t>
   </si>
   <si>
-    <t>FIELD</t>
-  </si>
-  <si>
     <t>物件番号</t>
   </si>
   <si>
@@ -796,6 +791,9 @@
     <t>001-001-003</t>
   </si>
   <si>
+    <t>IN_DB_003</t>
+  </si>
+  <si>
     <t>IN_FORM_003</t>
   </si>
   <si>
@@ -878,16 +876,19 @@
   </si>
   <si>
     <t>ホワイトボート</t>
-  </si>
-  <si>
-    <t>IN_DB_003</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="22">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="38">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -899,7 +900,6 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="宋体"/>
-      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -907,29 +907,19 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="DengXian"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <family val="3"/>
       <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
       <sz val="9"/>
       <color theme="1"/>
       <name val="Meiryo UI"/>
-      <family val="2"/>
       <charset val="128"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
-      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -958,7 +948,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="宋体"/>
-      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -978,7 +967,6 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="宋体"/>
-      <family val="3"/>
       <charset val="134"/>
     </font>
     <font>
@@ -986,7 +974,6 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="Meiryo UI"/>
-      <family val="2"/>
       <charset val="128"/>
     </font>
     <font>
@@ -994,7 +981,6 @@
       <sz val="10"/>
       <color theme="1"/>
       <name val="宋体"/>
-      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -1014,7 +1000,6 @@
       <sz val="10"/>
       <color theme="0"/>
       <name val="宋体"/>
-      <family val="3"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
@@ -1026,29 +1011,157 @@
       <charset val="128"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Meiryo UI"/>
-      <family val="2"/>
-      <charset val="128"/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
       <color theme="1"/>
       <name val="Meiryo UI"/>
-      <family val="2"/>
       <charset val="128"/>
     </font>
     <font>
-      <sz val="9"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="宋体"/>
-      <family val="3"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="14">
+  <fills count="45">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1063,19 +1176,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.59999389629810485"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.39991454817346722"/>
+        <fgColor theme="7" tint="0.399914548173467"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.39991454817346722"/>
+        <fgColor theme="9" tint="0.399914548173467"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1087,19 +1200,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.39997558519241921"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.59999389629810485"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="0" tint="-0.14993743705557422"/>
+        <fgColor theme="0" tint="-0.149937437055574"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1117,7 +1230,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39988402966399123"/>
+        <fgColor theme="8" tint="0.399884029663991"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1127,8 +1240,194 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="3">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -1164,12 +1463,254 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0"/>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="21" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="20" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="24" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="30" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="30" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="33" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="39" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="35" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="37" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="36" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="42" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="44" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="38" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="41" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="43" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="40" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1202,91 +1743,129 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="4" fillId="9" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="3" fillId="9" borderId="1" xfId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="8" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="12" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="9" borderId="1" xfId="14" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="14" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="10" fillId="11" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="9" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="15" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="17" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="10" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="11" fillId="13" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="10" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="19" fillId="9" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" quotePrefix="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" quotePrefix="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="標準 26" xfId="1"/>
+  <cellStyles count="50">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="货币[0]" xfId="1" builtinId="7"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="2" builtinId="38"/>
+    <cellStyle name="输入" xfId="3" builtinId="20"/>
+    <cellStyle name="货币" xfId="4" builtinId="4"/>
+    <cellStyle name="千位分隔[0]" xfId="5" builtinId="6"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="差" xfId="7" builtinId="27"/>
+    <cellStyle name="千位分隔" xfId="8" builtinId="3"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="9" builtinId="40"/>
+    <cellStyle name="超链接" xfId="10" builtinId="8"/>
+    <cellStyle name="百分比" xfId="11" builtinId="5"/>
+    <cellStyle name="已访问的超链接" xfId="12" builtinId="9"/>
+    <cellStyle name="注释" xfId="13" builtinId="10"/>
+    <cellStyle name="標準 26" xfId="14"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="15" builtinId="36"/>
+    <cellStyle name="标题 4" xfId="16" builtinId="19"/>
+    <cellStyle name="警告文本" xfId="17" builtinId="11"/>
+    <cellStyle name="标题" xfId="18" builtinId="15"/>
+    <cellStyle name="解释性文本" xfId="19" builtinId="53"/>
+    <cellStyle name="标题 1" xfId="20" builtinId="16"/>
+    <cellStyle name="标题 2" xfId="21" builtinId="17"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="22" builtinId="32"/>
+    <cellStyle name="标题 3" xfId="23" builtinId="18"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="24" builtinId="44"/>
+    <cellStyle name="输出" xfId="25" builtinId="21"/>
+    <cellStyle name="计算" xfId="26" builtinId="22"/>
+    <cellStyle name="检查单元格" xfId="27" builtinId="23"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="28" builtinId="50"/>
+    <cellStyle name="强调文字颜色 2" xfId="29" builtinId="33"/>
+    <cellStyle name="链接单元格" xfId="30" builtinId="24"/>
+    <cellStyle name="汇总" xfId="31" builtinId="25"/>
+    <cellStyle name="好" xfId="32" builtinId="26"/>
+    <cellStyle name="适中" xfId="33" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="34" builtinId="46"/>
+    <cellStyle name="强调文字颜色 1" xfId="35" builtinId="29"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="36" builtinId="30"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="37" builtinId="31"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="38" builtinId="34"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="39" builtinId="35"/>
+    <cellStyle name="强调文字颜色 3" xfId="40" builtinId="37"/>
+    <cellStyle name="强调文字颜色 4" xfId="41" builtinId="41"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="42" builtinId="42"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="43" builtinId="43"/>
+    <cellStyle name="强调文字颜色 5" xfId="44" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="45" builtinId="47"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="46" builtinId="48"/>
+    <cellStyle name="强调文字颜色 6" xfId="47" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="48" builtinId="51"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="49" builtinId="52"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="1">
     <dxf>
       <fill>
         <patternFill patternType="solid">
-          <bgColor theme="0" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor theme="0" tint="-0.24994659260841701"/>
+          <bgColor theme="0" tint="-0.249946592608417"/>
         </patternFill>
       </fill>
     </dxf>
@@ -1295,9 +1874,6 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1346,7 +1922,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1381,7 +1957,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1584,12 +2160,12 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A3:BV60"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -1605,8 +2181,8 @@
     <col min="6" max="16384" width="9" style="15"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:71" customFormat="1" ht="14.25">
-      <c r="A3" s="37" t="s">
+    <row r="3" customFormat="1" ht="14.25" spans="1:8">
+      <c r="A3" s="32" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="14" t="s">
@@ -1619,8 +2195,8 @@
       <c r="G3" s="15"/>
       <c r="H3" s="15"/>
     </row>
-    <row r="4" spans="1:71" customFormat="1" ht="14.25">
-      <c r="A4" s="37" t="s">
+    <row r="4" customFormat="1" ht="14.25" spans="1:8">
+      <c r="A4" s="32" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="14" t="s">
@@ -1633,8 +2209,8 @@
       <c r="G4" s="15"/>
       <c r="H4" s="15"/>
     </row>
-    <row r="5" spans="1:71" customFormat="1" ht="14.25">
-      <c r="A5" s="37" t="s">
+    <row r="5" customFormat="1" ht="14.25" spans="1:8">
+      <c r="A5" s="32" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="14" t="s">
@@ -1646,8 +2222,8 @@
       <c r="G5" s="15"/>
       <c r="H5" s="15"/>
     </row>
-    <row r="6" spans="1:71" customFormat="1" ht="14.25">
-      <c r="A6" s="37" t="s">
+    <row r="6" customFormat="1" ht="14.25" spans="1:8">
+      <c r="A6" s="32" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="14" t="s">
@@ -1660,7 +2236,7 @@
       <c r="G6" s="15"/>
       <c r="H6" s="15"/>
     </row>
-    <row r="7" spans="1:71" ht="14.25">
+    <row r="7" ht="14.25" spans="1:2">
       <c r="A7" s="32" t="s">
         <v>0</v>
       </c>
@@ -1668,7 +2244,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:71" ht="14.25">
+    <row r="8" ht="14.25" spans="1:7">
       <c r="A8" s="32" t="s">
         <v>0</v>
       </c>
@@ -1681,7 +2257,7 @@
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
     </row>
-    <row r="9" spans="1:71" ht="14.25">
+    <row r="9" ht="14.25" spans="1:7">
       <c r="A9" s="32" t="s">
         <v>0</v>
       </c>
@@ -1694,7 +2270,7 @@
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
     </row>
-    <row r="10" spans="1:71" ht="14.25">
+    <row r="10" ht="14.25" spans="1:7">
       <c r="A10" s="32" t="s">
         <v>0</v>
       </c>
@@ -1707,7 +2283,7 @@
       <c r="F10" s="14"/>
       <c r="G10" s="14"/>
     </row>
-    <row r="11" spans="1:71" ht="14.25">
+    <row r="11" ht="14.25" spans="1:7">
       <c r="A11" s="32" t="s">
         <v>0</v>
       </c>
@@ -1720,7 +2296,7 @@
       <c r="F11" s="14"/>
       <c r="G11" s="14"/>
     </row>
-    <row r="12" spans="1:71" ht="14.25">
+    <row r="12" ht="14.25" spans="1:7">
       <c r="A12" s="32" t="s">
         <v>0</v>
       </c>
@@ -1733,7 +2309,7 @@
       <c r="F12" s="14"/>
       <c r="G12" s="14"/>
     </row>
-    <row r="13" spans="1:71">
+    <row r="13" spans="1:7">
       <c r="A13" s="14"/>
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
@@ -1742,7 +2318,7 @@
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
     </row>
-    <row r="14" spans="1:71" customFormat="1" ht="13.5">
+    <row r="14" customFormat="1" ht="13.5" spans="1:7">
       <c r="A14" s="14"/>
       <c r="B14" s="14"/>
       <c r="C14" s="14"/>
@@ -1751,7 +2327,7 @@
       <c r="F14" s="14"/>
       <c r="G14" s="14"/>
     </row>
-    <row r="15" spans="1:71" s="13" customFormat="1" ht="12.75" customHeight="1">
+    <row r="15" s="13" customFormat="1" ht="12.75" customHeight="1" spans="1:2">
       <c r="A15" s="16" t="s">
         <v>11</v>
       </c>
@@ -1759,7 +2335,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:71" s="13" customFormat="1" ht="13.5">
+    <row r="16" s="13" customFormat="1" ht="13.5" spans="2:71">
       <c r="B16" s="17" t="s">
         <v>13</v>
       </c>
@@ -1833,7 +2409,7 @@
       <c r="BR16" s="18"/>
       <c r="BS16" s="18"/>
     </row>
-    <row r="17" spans="1:74" s="13" customFormat="1" ht="13.5">
+    <row r="17" s="13" customFormat="1" ht="13.5" spans="2:74">
       <c r="B17" s="19" t="s">
         <v>14</v>
       </c>
@@ -2054,7 +2630,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="1:74" s="13" customFormat="1" ht="16.5" customHeight="1">
+    <row r="18" s="13" customFormat="1" ht="16.5" customHeight="1" spans="1:74">
       <c r="A18" s="21"/>
       <c r="B18" s="22" t="s">
         <v>87</v>
@@ -2276,7 +2852,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="19" spans="1:74" customFormat="1" ht="13.5">
+    <row r="19" customFormat="1" ht="13.5" spans="2:74">
       <c r="B19" s="25"/>
       <c r="C19" s="25"/>
       <c r="D19" s="25"/>
@@ -2351,7 +2927,7 @@
       <c r="BU19" s="25"/>
       <c r="BV19" s="25"/>
     </row>
-    <row r="20" spans="1:74" customFormat="1" ht="13.5">
+    <row r="20" customFormat="1" ht="13.5" spans="1:7">
       <c r="A20" s="14"/>
       <c r="B20" s="14"/>
       <c r="C20" s="14"/>
@@ -2360,7 +2936,7 @@
       <c r="F20" s="14"/>
       <c r="G20" s="14"/>
     </row>
-    <row r="21" spans="1:74" customFormat="1" ht="13.5">
+    <row r="21" customFormat="1" ht="13.5" spans="1:7">
       <c r="A21" s="14"/>
       <c r="B21" s="14"/>
       <c r="C21" s="14"/>
@@ -2369,7 +2945,7 @@
       <c r="F21" s="14"/>
       <c r="G21" s="14"/>
     </row>
-    <row r="22" spans="1:74" customFormat="1" ht="13.5">
+    <row r="22" customFormat="1" ht="13.5" spans="1:7">
       <c r="A22" s="14"/>
       <c r="B22" s="14"/>
       <c r="C22" s="14"/>
@@ -2378,7 +2954,7 @@
       <c r="F22" s="14"/>
       <c r="G22" s="14"/>
     </row>
-    <row r="23" spans="1:74" customFormat="1" ht="13.5">
+    <row r="23" customFormat="1" ht="13.5" spans="1:7">
       <c r="A23" s="14"/>
       <c r="B23" s="14"/>
       <c r="C23" s="14"/>
@@ -2387,7 +2963,7 @@
       <c r="F23" s="14"/>
       <c r="G23" s="14"/>
     </row>
-    <row r="24" spans="1:74" s="14" customFormat="1" ht="14.25">
+    <row r="24" s="14" customFormat="1" ht="14.25" spans="1:2">
       <c r="A24" s="32" t="s">
         <v>11</v>
       </c>
@@ -2395,7 +2971,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="25" spans="1:74" s="14" customFormat="1">
+    <row r="25" s="14" customFormat="1" spans="2:19">
       <c r="B25" s="33" t="s">
         <v>106</v>
       </c>
@@ -2451,7 +3027,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="26" spans="1:74" s="14" customFormat="1">
+    <row r="26" s="14" customFormat="1" spans="2:19">
       <c r="B26" s="20" t="s">
         <v>108</v>
       </c>
@@ -2507,7 +3083,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="27" spans="1:74" s="14" customFormat="1">
+    <row r="27" s="14" customFormat="1" spans="2:19">
       <c r="B27" s="23" t="s">
         <v>102</v>
       </c>
@@ -2563,7 +3139,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="28" spans="1:74" s="14" customFormat="1">
+    <row r="28" s="14" customFormat="1" spans="2:19">
       <c r="B28" s="23" t="s">
         <v>99</v>
       </c>
@@ -2619,7 +3195,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="29" spans="1:74" s="14" customFormat="1">
+    <row r="29" s="14" customFormat="1" spans="2:19">
       <c r="B29" s="23" t="s">
         <v>126</v>
       </c>
@@ -2675,7 +3251,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="30" spans="1:74" s="14" customFormat="1">
+    <row r="30" s="14" customFormat="1" spans="2:19">
       <c r="B30" s="23" t="s">
         <v>129</v>
       </c>
@@ -2731,7 +3307,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="31" spans="1:74" s="14" customFormat="1">
+    <row r="31" s="14" customFormat="1" spans="2:19">
       <c r="B31" s="23" t="s">
         <v>132</v>
       </c>
@@ -2787,7 +3363,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="32" spans="1:74" s="14" customFormat="1">
+    <row r="32" s="14" customFormat="1" spans="2:19">
       <c r="B32" s="23" t="s">
         <v>104</v>
       </c>
@@ -2843,7 +3419,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="33" spans="1:19" s="14" customFormat="1">
+    <row r="33" s="14" customFormat="1" spans="2:19">
       <c r="B33" s="23" t="s">
         <v>137</v>
       </c>
@@ -2899,8 +3475,8 @@
         <v>89</v>
       </c>
     </row>
-    <row r="34" spans="1:19" s="14" customFormat="1"/>
-    <row r="36" spans="1:19" ht="14.25">
+    <row r="34" s="14" customFormat="1"/>
+    <row r="36" ht="14.25" spans="1:7">
       <c r="A36" s="32" t="s">
         <v>11</v>
       </c>
@@ -2913,7 +3489,7 @@
       <c r="F36" s="14"/>
       <c r="G36" s="14"/>
     </row>
-    <row r="37" spans="1:19">
+    <row r="37" spans="2:7">
       <c r="B37" s="33" t="s">
         <v>141</v>
       </c>
@@ -2933,7 +3509,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="38" spans="1:19">
+    <row r="38" spans="1:7">
       <c r="A38" s="14"/>
       <c r="B38" s="20" t="s">
         <v>108</v>
@@ -2954,7 +3530,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="39" spans="1:19">
+    <row r="39" spans="1:7">
       <c r="A39" s="14"/>
       <c r="B39" s="23" t="s">
         <v>102</v>
@@ -2975,7 +3551,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="42" spans="1:19" ht="14.25">
+    <row r="42" ht="14.25" spans="1:10">
       <c r="A42" s="32" t="s">
         <v>11</v>
       </c>
@@ -2991,7 +3567,7 @@
       <c r="I42" s="14"/>
       <c r="J42" s="14"/>
     </row>
-    <row r="43" spans="1:19">
+    <row r="43" spans="2:10">
       <c r="B43" s="33" t="s">
         <v>144</v>
       </c>
@@ -3020,7 +3596,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="44" spans="1:19">
+    <row r="44" spans="1:10">
       <c r="A44" s="14"/>
       <c r="B44" s="20" t="s">
         <v>108</v>
@@ -3050,7 +3626,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="45" spans="1:19">
+    <row r="45" spans="1:10">
       <c r="A45" s="14"/>
       <c r="B45" s="23" t="s">
         <v>102</v>
@@ -3080,7 +3656,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="46" spans="1:19">
+    <row r="46" spans="1:10">
       <c r="A46" s="14"/>
       <c r="B46" s="23" t="s">
         <v>99</v>
@@ -3110,7 +3686,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="47" spans="1:19">
+    <row r="47" spans="1:10">
       <c r="A47" s="14"/>
       <c r="B47" s="23" t="s">
         <v>126</v>
@@ -3140,7 +3716,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="48" spans="1:19">
+    <row r="48" spans="1:10">
       <c r="A48" s="14"/>
       <c r="B48" s="23" t="s">
         <v>129</v>
@@ -3170,7 +3746,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="49" spans="1:13">
+    <row r="49" spans="1:10">
       <c r="A49" s="14"/>
       <c r="B49" s="23" t="s">
         <v>132</v>
@@ -3200,7 +3776,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="50" spans="1:13">
+    <row r="50" spans="1:10">
       <c r="A50" s="14"/>
       <c r="B50" s="23" t="s">
         <v>104</v>
@@ -3230,7 +3806,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="51" spans="1:13">
+    <row r="51" spans="1:10">
       <c r="A51" s="14"/>
       <c r="B51" s="23" t="s">
         <v>137</v>
@@ -3260,7 +3836,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="54" spans="1:13" s="14" customFormat="1" ht="14.25">
+    <row r="54" s="14" customFormat="1" ht="14.25" spans="1:2">
       <c r="A54" s="32" t="s">
         <v>11</v>
       </c>
@@ -3268,7 +3844,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="55" spans="1:13" s="14" customFormat="1">
+    <row r="55" s="14" customFormat="1" spans="2:13">
       <c r="B55" s="33" t="s">
         <v>150</v>
       </c>
@@ -3306,7 +3882,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="56" spans="1:13" s="14" customFormat="1">
+    <row r="56" s="14" customFormat="1" spans="2:13">
       <c r="B56" s="20" t="s">
         <v>108</v>
       </c>
@@ -3344,7 +3920,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="57" spans="1:13" s="14" customFormat="1">
+    <row r="57" s="14" customFormat="1" spans="2:13">
       <c r="B57" s="23" t="s">
         <v>102</v>
       </c>
@@ -3382,7 +3958,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="58" spans="1:13" s="14" customFormat="1">
+    <row r="58" s="14" customFormat="1" spans="2:13">
       <c r="B58" s="23" t="s">
         <v>99</v>
       </c>
@@ -3420,7 +3996,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="59" spans="1:13" s="14" customFormat="1">
+    <row r="59" s="14" customFormat="1" spans="2:13">
       <c r="B59" s="23" t="s">
         <v>126</v>
       </c>
@@ -3458,28 +4034,29 @@
         <v>89</v>
       </c>
     </row>
-    <row r="60" spans="1:13" s="14" customFormat="1"/>
+    <row r="60" s="14" customFormat="1"/>
   </sheetData>
-  <phoneticPr fontId="21" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A2:BV8"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="U48" sqref="U48"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:74" s="13" customFormat="1" ht="12.75" customHeight="1">
+    <row r="2" s="13" customFormat="1" ht="12.75" customHeight="1" spans="1:2">
       <c r="A2" s="16" t="s">
         <v>11</v>
       </c>
@@ -3487,7 +4064,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:74" s="13" customFormat="1">
+    <row r="3" s="13" customFormat="1" spans="2:71">
       <c r="B3" s="17" t="s">
         <v>13</v>
       </c>
@@ -3561,7 +4138,7 @@
       <c r="BR3" s="18"/>
       <c r="BS3" s="18"/>
     </row>
-    <row r="4" spans="1:74" s="13" customFormat="1">
+    <row r="4" s="13" customFormat="1" spans="2:74">
       <c r="B4" s="19" t="s">
         <v>14</v>
       </c>
@@ -3782,7 +4359,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:74" s="13" customFormat="1" ht="16.5" customHeight="1">
+    <row r="5" s="13" customFormat="1" ht="16.5" customHeight="1" spans="1:74">
       <c r="A5" s="21"/>
       <c r="B5" s="22" t="s">
         <v>169</v>
@@ -4004,7 +4581,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:74">
+    <row r="6" spans="2:74">
       <c r="B6" s="25"/>
       <c r="C6" s="25"/>
       <c r="D6" s="25"/>
@@ -4079,16 +4656,17 @@
       <c r="BU6" s="25"/>
       <c r="BV6" s="25"/>
     </row>
-    <row r="7" spans="1:74" s="14" customFormat="1" ht="12"/>
-    <row r="8" spans="1:74" s="15" customFormat="1" ht="12"/>
+    <row r="7" s="14" customFormat="1" ht="12"/>
+    <row r="8" s="15" customFormat="1" ht="12"/>
   </sheetData>
-  <phoneticPr fontId="21" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A2:S44"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -4104,7 +4682,7 @@
     <col min="6" max="16384" width="9" style="15"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:19" ht="14.25">
+    <row r="2" ht="14.25" spans="1:7">
       <c r="A2" s="32" t="s">
         <v>0</v>
       </c>
@@ -4117,7 +4695,7 @@
       <c r="F2" s="14"/>
       <c r="G2" s="14"/>
     </row>
-    <row r="3" spans="1:19" ht="14.25">
+    <row r="3" ht="14.25" spans="1:7">
       <c r="A3" s="32" t="s">
         <v>0</v>
       </c>
@@ -4130,7 +4708,7 @@
       <c r="F3" s="14"/>
       <c r="G3" s="14"/>
     </row>
-    <row r="4" spans="1:19" ht="14.25">
+    <row r="4" ht="14.25" spans="1:7">
       <c r="A4" s="32" t="s">
         <v>0</v>
       </c>
@@ -4143,7 +4721,7 @@
       <c r="F4" s="14"/>
       <c r="G4" s="14"/>
     </row>
-    <row r="5" spans="1:19" ht="14.25">
+    <row r="5" ht="14.25" spans="1:7">
       <c r="A5" s="32" t="s">
         <v>0</v>
       </c>
@@ -4156,7 +4734,7 @@
       <c r="F5" s="14"/>
       <c r="G5" s="14"/>
     </row>
-    <row r="6" spans="1:19" ht="14.25">
+    <row r="6" ht="14.25" spans="1:7">
       <c r="A6" s="32" t="s">
         <v>0</v>
       </c>
@@ -4169,7 +4747,7 @@
       <c r="F6" s="14"/>
       <c r="G6" s="14"/>
     </row>
-    <row r="7" spans="1:19">
+    <row r="7" spans="1:7">
       <c r="A7" s="14"/>
       <c r="B7" s="14"/>
       <c r="C7" s="14"/>
@@ -4178,7 +4756,7 @@
       <c r="F7" s="14"/>
       <c r="G7" s="14"/>
     </row>
-    <row r="8" spans="1:19" s="14" customFormat="1" ht="14.25">
+    <row r="8" s="14" customFormat="1" ht="14.25" spans="1:2">
       <c r="A8" s="32" t="s">
         <v>11</v>
       </c>
@@ -4186,7 +4764,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="9" spans="1:19" s="14" customFormat="1">
+    <row r="9" s="14" customFormat="1" spans="2:19">
       <c r="B9" s="33" t="s">
         <v>106</v>
       </c>
@@ -4242,7 +4820,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="10" spans="1:19" s="14" customFormat="1">
+    <row r="10" s="14" customFormat="1" spans="2:19">
       <c r="B10" s="20" t="s">
         <v>108</v>
       </c>
@@ -4298,7 +4876,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="11" spans="1:19" s="14" customFormat="1">
+    <row r="11" s="14" customFormat="1" spans="2:19">
       <c r="B11" s="23" t="s">
         <v>102</v>
       </c>
@@ -4354,7 +4932,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:19" s="14" customFormat="1">
+    <row r="12" s="14" customFormat="1" spans="2:19">
       <c r="B12" s="23" t="s">
         <v>99</v>
       </c>
@@ -4410,7 +4988,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="13" spans="1:19" s="14" customFormat="1">
+    <row r="13" s="14" customFormat="1" spans="2:19">
       <c r="B13" s="23" t="s">
         <v>126</v>
       </c>
@@ -4466,7 +5044,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="14" spans="1:19" s="14" customFormat="1">
+    <row r="14" s="14" customFormat="1" spans="2:19">
       <c r="B14" s="23" t="s">
         <v>129</v>
       </c>
@@ -4522,7 +5100,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:19" s="14" customFormat="1">
+    <row r="15" s="14" customFormat="1" spans="2:19">
       <c r="B15" s="23" t="s">
         <v>132</v>
       </c>
@@ -4578,7 +5156,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:19" s="14" customFormat="1">
+    <row r="16" s="14" customFormat="1" spans="2:19">
       <c r="B16" s="23" t="s">
         <v>104</v>
       </c>
@@ -4634,7 +5212,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="1:19" s="14" customFormat="1">
+    <row r="17" s="14" customFormat="1" spans="2:19">
       <c r="B17" s="23" t="s">
         <v>137</v>
       </c>
@@ -4690,8 +5268,8 @@
         <v>89</v>
       </c>
     </row>
-    <row r="18" spans="1:19" s="14" customFormat="1"/>
-    <row r="20" spans="1:19" ht="14.25">
+    <row r="18" s="14" customFormat="1"/>
+    <row r="20" ht="14.25" spans="1:7">
       <c r="A20" s="32" t="s">
         <v>11</v>
       </c>
@@ -4704,7 +5282,7 @@
       <c r="F20" s="14"/>
       <c r="G20" s="14"/>
     </row>
-    <row r="21" spans="1:19">
+    <row r="21" spans="2:7">
       <c r="B21" s="33" t="s">
         <v>141</v>
       </c>
@@ -4724,7 +5302,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="22" spans="1:19">
+    <row r="22" spans="1:7">
       <c r="A22" s="14"/>
       <c r="B22" s="20" t="s">
         <v>108</v>
@@ -4745,7 +5323,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:19">
+    <row r="23" spans="1:7">
       <c r="A23" s="14"/>
       <c r="B23" s="23" t="s">
         <v>102</v>
@@ -4766,7 +5344,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="26" spans="1:19" ht="14.25">
+    <row r="26" ht="14.25" spans="1:10">
       <c r="A26" s="32" t="s">
         <v>11</v>
       </c>
@@ -4782,7 +5360,7 @@
       <c r="I26" s="14"/>
       <c r="J26" s="14"/>
     </row>
-    <row r="27" spans="1:19">
+    <row r="27" spans="2:10">
       <c r="B27" s="33" t="s">
         <v>144</v>
       </c>
@@ -4811,7 +5389,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="1:19">
+    <row r="28" spans="1:10">
       <c r="A28" s="14"/>
       <c r="B28" s="20" t="s">
         <v>108</v>
@@ -4841,7 +5419,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="29" spans="1:19">
+    <row r="29" spans="1:10">
       <c r="A29" s="14"/>
       <c r="B29" s="23" t="s">
         <v>102</v>
@@ -4871,7 +5449,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="30" spans="1:19">
+    <row r="30" spans="1:10">
       <c r="A30" s="14"/>
       <c r="B30" s="23" t="s">
         <v>99</v>
@@ -4901,7 +5479,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="31" spans="1:19">
+    <row r="31" spans="1:10">
       <c r="A31" s="14"/>
       <c r="B31" s="23" t="s">
         <v>126</v>
@@ -4931,7 +5509,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="32" spans="1:19">
+    <row r="32" spans="1:10">
       <c r="A32" s="14"/>
       <c r="B32" s="23" t="s">
         <v>129</v>
@@ -4961,7 +5539,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="33" spans="1:13">
+    <row r="33" spans="1:10">
       <c r="A33" s="14"/>
       <c r="B33" s="23" t="s">
         <v>132</v>
@@ -4991,7 +5569,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="34" spans="1:13">
+    <row r="34" spans="1:10">
       <c r="A34" s="14"/>
       <c r="B34" s="23" t="s">
         <v>104</v>
@@ -5021,7 +5599,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="35" spans="1:13">
+    <row r="35" spans="1:10">
       <c r="A35" s="14"/>
       <c r="B35" s="23" t="s">
         <v>137</v>
@@ -5051,7 +5629,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="38" spans="1:13" s="14" customFormat="1" ht="14.25">
+    <row r="38" s="14" customFormat="1" ht="14.25" spans="1:2">
       <c r="A38" s="32" t="s">
         <v>11</v>
       </c>
@@ -5059,7 +5637,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="39" spans="1:13" s="14" customFormat="1">
+    <row r="39" s="14" customFormat="1" spans="2:13">
       <c r="B39" s="33" t="s">
         <v>150</v>
       </c>
@@ -5097,7 +5675,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="40" spans="1:13" s="14" customFormat="1">
+    <row r="40" s="14" customFormat="1" spans="2:13">
       <c r="B40" s="20" t="s">
         <v>108</v>
       </c>
@@ -5135,7 +5713,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="41" spans="1:13" s="14" customFormat="1">
+    <row r="41" s="14" customFormat="1" spans="2:13">
       <c r="B41" s="23" t="s">
         <v>102</v>
       </c>
@@ -5173,7 +5751,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="42" spans="1:13" s="14" customFormat="1">
+    <row r="42" s="14" customFormat="1" spans="2:13">
       <c r="B42" s="23" t="s">
         <v>99</v>
       </c>
@@ -5211,7 +5789,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="43" spans="1:13" s="14" customFormat="1">
+    <row r="43" s="14" customFormat="1" spans="2:13">
       <c r="B43" s="23" t="s">
         <v>126</v>
       </c>
@@ -5249,23 +5827,24 @@
         <v>89</v>
       </c>
     </row>
-    <row r="44" spans="1:13" s="14" customFormat="1"/>
+    <row r="44" s="14" customFormat="1"/>
   </sheetData>
-  <phoneticPr fontId="21" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="I40" sqref="I40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="9" style="15" customWidth="1"/>
     <col min="2" max="2" width="15.625" style="15" customWidth="1"/>
@@ -5275,15 +5854,15 @@
     <col min="6" max="16384" width="9" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="12" customHeight="1">
+    <row r="1" customHeight="1" spans="1:2">
       <c r="A1" s="27" t="s">
         <v>164</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="37" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="12" customHeight="1">
+    <row r="4" customHeight="1" spans="1:2">
       <c r="A4" s="27" t="s">
         <v>166</v>
       </c>
@@ -5291,7 +5870,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="14.25">
+    <row r="5" ht="14.25" spans="1:2">
       <c r="A5" s="27" t="s">
         <v>166</v>
       </c>
@@ -5299,14 +5878,14 @@
         <v>168</v>
       </c>
     </row>
-    <row r="7" spans="1:5" customFormat="1" ht="13.5">
+    <row r="7" customFormat="1" ht="13.5" spans="1:5">
       <c r="A7" s="15"/>
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
     </row>
-    <row r="9" spans="1:5" ht="14.25">
+    <row r="9" ht="14.25" spans="1:2">
       <c r="A9" s="27" t="s">
         <v>166</v>
       </c>
@@ -5314,7 +5893,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="12" customHeight="1">
+    <row r="12" customHeight="1" spans="1:2">
       <c r="A12" s="27" t="s">
         <v>166</v>
       </c>
@@ -5323,26 +5902,27 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="21" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A2:BV8"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="T39" sqref="T39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:74" s="13" customFormat="1" ht="12.75" customHeight="1">
+    <row r="2" s="13" customFormat="1" ht="12.75" customHeight="1" spans="1:2">
       <c r="A2" s="16" t="s">
         <v>11</v>
       </c>
@@ -5350,7 +5930,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:74" s="13" customFormat="1">
+    <row r="3" s="13" customFormat="1" spans="2:71">
       <c r="B3" s="17" t="s">
         <v>13</v>
       </c>
@@ -5424,7 +6004,7 @@
       <c r="BR3" s="18"/>
       <c r="BS3" s="18"/>
     </row>
-    <row r="4" spans="1:74" s="13" customFormat="1">
+    <row r="4" s="13" customFormat="1" spans="2:74">
       <c r="B4" s="19" t="s">
         <v>14</v>
       </c>
@@ -5645,7 +6225,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:74" s="13" customFormat="1" ht="16.5" customHeight="1">
+    <row r="5" s="13" customFormat="1" ht="16.5" customHeight="1" spans="1:74">
       <c r="A5" s="21"/>
       <c r="B5" s="22" t="s">
         <v>169</v>
@@ -5867,7 +6447,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:74">
+    <row r="6" spans="2:74">
       <c r="B6" s="25"/>
       <c r="C6" s="25"/>
       <c r="D6" s="25"/>
@@ -5942,23 +6522,24 @@
       <c r="BU6" s="25"/>
       <c r="BV6" s="25"/>
     </row>
-    <row r="7" spans="1:74" s="14" customFormat="1" ht="12"/>
-    <row r="8" spans="1:74" s="15" customFormat="1" ht="12"/>
+    <row r="7" s="14" customFormat="1" ht="12"/>
+    <row r="8" s="15" customFormat="1" ht="12"/>
   </sheetData>
-  <phoneticPr fontId="21" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:E22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="9" style="15" customWidth="1"/>
     <col min="2" max="2" width="15.625" style="15" customWidth="1"/>
@@ -5968,15 +6549,15 @@
     <col min="6" max="16384" width="9" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="12" customHeight="1">
+    <row r="1" customHeight="1" spans="1:2">
       <c r="A1" s="27" t="s">
         <v>164</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="37" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="12" customHeight="1">
+    <row r="4" customHeight="1" spans="1:2">
       <c r="A4" s="27" t="s">
         <v>166</v>
       </c>
@@ -5984,7 +6565,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="14.25">
+    <row r="5" ht="14.25" spans="1:2">
       <c r="A5" s="27" t="s">
         <v>166</v>
       </c>
@@ -5992,14 +6573,14 @@
         <v>168</v>
       </c>
     </row>
-    <row r="7" spans="1:5" customFormat="1" ht="13.5">
+    <row r="7" customFormat="1" ht="13.5" spans="1:5">
       <c r="A7" s="15"/>
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
     </row>
-    <row r="9" spans="1:5" ht="14.25">
+    <row r="9" ht="14.25" spans="1:2">
       <c r="A9" s="27" t="s">
         <v>166</v>
       </c>
@@ -6007,7 +6588,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="12" customHeight="1">
+    <row r="12" customHeight="1" spans="1:2">
       <c r="A12" s="27" t="s">
         <v>166</v>
       </c>
@@ -6015,18 +6596,18 @@
         <v>224</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="14.25">
+    <row r="13" ht="14.25" spans="1:1">
       <c r="A13" s="27"/>
     </row>
-    <row r="16" spans="1:5" ht="14.25">
+    <row r="16" ht="14.25" spans="1:2">
       <c r="A16" s="27" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="14.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="17" ht="14.25" spans="1:4">
       <c r="A17" s="27"/>
       <c r="B17" s="28" t="s">
         <v>176</v>
@@ -6038,21 +6619,21 @@
         <v>178</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="14.25">
+    <row r="18" ht="14.25" spans="1:4">
       <c r="A18" s="27" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B18" s="29" t="s">
         <v>225</v>
       </c>
-      <c r="C18" s="39" t="s">
+      <c r="C18" s="38" t="s">
         <v>226</v>
       </c>
       <c r="D18" s="31" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="14.25">
+    <row r="22" ht="14.25" spans="1:2">
       <c r="A22" s="27" t="s">
         <v>166</v>
       </c>
@@ -6061,26 +6642,27 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="21" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A2:BV8"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="U57" sqref="U57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:74" s="13" customFormat="1" ht="12.75" customHeight="1">
+    <row r="2" s="13" customFormat="1" ht="12.75" customHeight="1" spans="1:2">
       <c r="A2" s="16" t="s">
         <v>11</v>
       </c>
@@ -6088,7 +6670,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:74" s="13" customFormat="1">
+    <row r="3" s="13" customFormat="1" spans="2:71">
       <c r="B3" s="17" t="s">
         <v>13</v>
       </c>
@@ -6162,7 +6744,7 @@
       <c r="BR3" s="18"/>
       <c r="BS3" s="18"/>
     </row>
-    <row r="4" spans="1:74" s="13" customFormat="1">
+    <row r="4" s="13" customFormat="1" spans="2:74">
       <c r="B4" s="19" t="s">
         <v>14</v>
       </c>
@@ -6383,7 +6965,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:74" s="13" customFormat="1" ht="16.5" customHeight="1">
+    <row r="5" s="13" customFormat="1" ht="16.5" customHeight="1" spans="1:74">
       <c r="A5" s="21"/>
       <c r="B5" s="22" t="s">
         <v>169</v>
@@ -6605,7 +7187,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:74">
+    <row r="6" spans="2:74">
       <c r="B6" s="25"/>
       <c r="C6" s="25"/>
       <c r="D6" s="25"/>
@@ -6680,23 +7262,24 @@
       <c r="BU6" s="25"/>
       <c r="BV6" s="25"/>
     </row>
-    <row r="7" spans="1:74" s="14" customFormat="1" ht="12"/>
-    <row r="8" spans="1:74" s="15" customFormat="1" ht="12"/>
+    <row r="7" s="14" customFormat="1" ht="12"/>
+    <row r="8" s="15" customFormat="1" ht="12"/>
   </sheetData>
-  <phoneticPr fontId="21" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:E22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13:XFD13"/>
+      <selection activeCell="A13" sqref="$A13:$XFD13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="9" style="15" customWidth="1"/>
     <col min="2" max="2" width="15.625" style="15" customWidth="1"/>
@@ -6706,15 +7289,15 @@
     <col min="6" max="16384" width="9" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="12" customHeight="1">
+    <row r="1" customHeight="1" spans="1:2">
       <c r="A1" s="27" t="s">
         <v>164</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="37" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="12" customHeight="1">
+    <row r="4" customHeight="1" spans="1:2">
       <c r="A4" s="27" t="s">
         <v>166</v>
       </c>
@@ -6722,7 +7305,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="14.25">
+    <row r="5" ht="14.25" spans="1:2">
       <c r="A5" s="27" t="s">
         <v>166</v>
       </c>
@@ -6730,14 +7313,14 @@
         <v>168</v>
       </c>
     </row>
-    <row r="7" spans="1:5" customFormat="1" ht="13.5">
+    <row r="7" customFormat="1" ht="13.5" spans="1:5">
       <c r="A7" s="15"/>
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
     </row>
-    <row r="9" spans="1:5" ht="14.25">
+    <row r="9" ht="14.25" spans="1:2">
       <c r="A9" s="27" t="s">
         <v>166</v>
       </c>
@@ -6745,7 +7328,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="12" customHeight="1">
+    <row r="12" customHeight="1" spans="1:2">
       <c r="A12" s="27" t="s">
         <v>166</v>
       </c>
@@ -6753,18 +7336,18 @@
         <v>228</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="14.25">
+    <row r="13" ht="14.25" spans="1:1">
       <c r="A13" s="27"/>
     </row>
-    <row r="16" spans="1:5" ht="14.25">
+    <row r="16" ht="14.25" spans="1:2">
       <c r="A16" s="27" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B16" s="15" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" ht="14.25">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="17" ht="14.25" spans="1:4">
       <c r="A17" s="27"/>
       <c r="B17" s="28" t="s">
         <v>176</v>
@@ -6776,21 +7359,21 @@
         <v>178</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="14.25">
+    <row r="18" ht="14.25" spans="1:4">
       <c r="A18" s="27" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B18" s="29" t="s">
         <v>225</v>
       </c>
-      <c r="C18" s="39" t="s">
+      <c r="C18" s="38" t="s">
         <v>229</v>
       </c>
       <c r="D18" s="31" t="s">
         <v>227</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="14.25">
+    <row r="22" ht="14.25" spans="1:2">
       <c r="A22" s="27" t="s">
         <v>166</v>
       </c>
@@ -6799,26 +7382,27 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="21" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A2:BV8"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="U52" sqref="U52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:74" s="13" customFormat="1" ht="12.75" customHeight="1">
+    <row r="2" s="13" customFormat="1" ht="12.75" customHeight="1" spans="1:2">
       <c r="A2" s="16" t="s">
         <v>11</v>
       </c>
@@ -6826,7 +7410,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:74" s="13" customFormat="1">
+    <row r="3" s="13" customFormat="1" spans="2:71">
       <c r="B3" s="17" t="s">
         <v>13</v>
       </c>
@@ -6900,7 +7484,7 @@
       <c r="BR3" s="18"/>
       <c r="BS3" s="18"/>
     </row>
-    <row r="4" spans="1:74" s="13" customFormat="1">
+    <row r="4" s="13" customFormat="1" spans="2:74">
       <c r="B4" s="19" t="s">
         <v>14</v>
       </c>
@@ -7121,7 +7705,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:74" s="13" customFormat="1" ht="16.5" customHeight="1">
+    <row r="5" s="13" customFormat="1" ht="16.5" customHeight="1" spans="1:74">
       <c r="A5" s="21"/>
       <c r="B5" s="22" t="s">
         <v>169</v>
@@ -7343,7 +7927,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:74">
+    <row r="6" spans="2:74">
       <c r="B6" s="25"/>
       <c r="C6" s="25"/>
       <c r="D6" s="25"/>
@@ -7418,23 +8002,24 @@
       <c r="BU6" s="25"/>
       <c r="BV6" s="25"/>
     </row>
-    <row r="7" spans="1:74" s="14" customFormat="1" ht="12"/>
-    <row r="8" spans="1:74" s="15" customFormat="1" ht="12"/>
+    <row r="7" s="14" customFormat="1" ht="12"/>
+    <row r="8" s="15" customFormat="1" ht="12"/>
   </sheetData>
-  <phoneticPr fontId="21" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12" outlineLevelRow="6" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="9" style="15" customWidth="1"/>
     <col min="2" max="2" width="15.625" style="15" customWidth="1"/>
@@ -7444,15 +8029,15 @@
     <col min="6" max="16384" width="9" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="12" customHeight="1">
+    <row r="1" customHeight="1" spans="1:2">
       <c r="A1" s="27" t="s">
         <v>164</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="37" t="s">
         <v>230</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="12" customHeight="1">
+    <row r="4" customHeight="1" spans="1:2">
       <c r="A4" s="27" t="s">
         <v>166</v>
       </c>
@@ -7460,7 +8045,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="14.25">
+    <row r="5" ht="14.25" spans="1:2">
       <c r="A5" s="27" t="s">
         <v>166</v>
       </c>
@@ -7468,7 +8053,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="7" spans="1:5" customFormat="1" ht="13.5">
+    <row r="7" customFormat="1" ht="13.5" spans="1:5">
       <c r="A7" s="15"/>
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
@@ -7476,26 +8061,27 @@
       <c r="E7" s="15"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="21" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A2:BV8"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G53" sqref="G53"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:74" s="13" customFormat="1" ht="12.75" customHeight="1">
+    <row r="2" s="13" customFormat="1" ht="12.75" customHeight="1" spans="1:2">
       <c r="A2" s="16" t="s">
         <v>11</v>
       </c>
@@ -7503,7 +8089,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:74" s="13" customFormat="1">
+    <row r="3" s="13" customFormat="1" spans="2:71">
       <c r="B3" s="17" t="s">
         <v>13</v>
       </c>
@@ -7577,7 +8163,7 @@
       <c r="BR3" s="18"/>
       <c r="BS3" s="18"/>
     </row>
-    <row r="4" spans="1:74" s="13" customFormat="1">
+    <row r="4" s="13" customFormat="1" spans="2:74">
       <c r="B4" s="19" t="s">
         <v>14</v>
       </c>
@@ -7798,7 +8384,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:74" s="13" customFormat="1" ht="16.5" customHeight="1">
+    <row r="5" s="13" customFormat="1" ht="16.5" customHeight="1" spans="1:74">
       <c r="A5" s="21"/>
       <c r="B5" s="22" t="s">
         <v>169</v>
@@ -8020,7 +8606,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:74">
+    <row r="6" spans="2:74">
       <c r="B6" s="25"/>
       <c r="C6" s="25"/>
       <c r="D6" s="25"/>
@@ -8095,23 +8681,24 @@
       <c r="BU6" s="25"/>
       <c r="BV6" s="25"/>
     </row>
-    <row r="7" spans="1:74" s="14" customFormat="1" ht="12"/>
-    <row r="8" spans="1:74" s="15" customFormat="1" ht="12"/>
+    <row r="7" s="14" customFormat="1" ht="12"/>
+    <row r="8" s="15" customFormat="1" ht="12"/>
   </sheetData>
-  <phoneticPr fontId="21" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12" outlineLevelRow="6" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="9" style="15" customWidth="1"/>
     <col min="2" max="2" width="15.625" style="15" customWidth="1"/>
@@ -8121,15 +8708,15 @@
     <col min="6" max="16384" width="9" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="12" customHeight="1">
+    <row r="1" customHeight="1" spans="1:2">
       <c r="A1" s="27" t="s">
         <v>164</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="37" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="12" customHeight="1">
+    <row r="4" customHeight="1" spans="1:2">
       <c r="A4" s="27" t="s">
         <v>166</v>
       </c>
@@ -8137,7 +8724,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="14.25">
+    <row r="5" ht="14.25" spans="1:2">
       <c r="A5" s="27" t="s">
         <v>166</v>
       </c>
@@ -8145,7 +8732,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="7" spans="1:5" customFormat="1" ht="13.5">
+    <row r="7" customFormat="1" ht="13.5" spans="1:5">
       <c r="A7" s="15"/>
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
@@ -8153,14 +8740,15 @@
       <c r="E7" s="15"/>
     </row>
   </sheetData>
-  <phoneticPr fontId="21" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="B4:J12"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -8252,70 +8840,70 @@
         <v>251</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>280</v>
+        <v>252</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="I7" s="11"/>
       <c r="J7" s="12" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
     </row>
     <row r="8" spans="2:10">
       <c r="B8" s="1" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="I8" s="11"/>
       <c r="J8" s="12" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
     </row>
     <row r="9" spans="2:10">
       <c r="B9" s="1" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="I9" s="11"/>
       <c r="J9" s="12" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
     </row>
     <row r="10" spans="2:10">
       <c r="B10" s="1" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="F10" s="1" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="I10" s="11"/>
       <c r="J10" s="12" t="s">
@@ -8324,46 +8912,45 @@
     </row>
     <row r="11" spans="2:10">
       <c r="B11" s="1" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="E11" s="1" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="F11" s="1" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="I11" s="11"/>
       <c r="J11" s="12" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
     </row>
     <row r="12" spans="2:10">
       <c r="B12" s="1" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="E12" s="1" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="F12" s="1" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="I12" s="10" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="J12" s="10" t="s">
         <v>245</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="21" type="noConversion"/>
   <conditionalFormatting sqref="I5:J5">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>$M5="完了"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -8372,25 +8959,27 @@
       <formula>$M12="完了"</formula>
     </cfRule>
   </conditionalFormatting>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A2:BV8"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="G42" sqref="G42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:74" s="13" customFormat="1" ht="12.75" customHeight="1">
+    <row r="2" s="13" customFormat="1" ht="12.75" customHeight="1" spans="1:2">
       <c r="A2" s="16" t="s">
         <v>11</v>
       </c>
@@ -8398,7 +8987,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:74" s="13" customFormat="1">
+    <row r="3" s="13" customFormat="1" spans="2:71">
       <c r="B3" s="17" t="s">
         <v>13</v>
       </c>
@@ -8472,7 +9061,7 @@
       <c r="BR3" s="18"/>
       <c r="BS3" s="18"/>
     </row>
-    <row r="4" spans="1:74" s="13" customFormat="1">
+    <row r="4" s="13" customFormat="1" spans="2:74">
       <c r="B4" s="19" t="s">
         <v>14</v>
       </c>
@@ -8693,7 +9282,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:74" s="13" customFormat="1" ht="16.5" customHeight="1">
+    <row r="5" s="13" customFormat="1" ht="16.5" customHeight="1" spans="1:74">
       <c r="A5" s="21"/>
       <c r="B5" s="22" t="s">
         <v>169</v>
@@ -8915,7 +9504,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:74">
+    <row r="6" spans="2:74">
       <c r="B6" s="25"/>
       <c r="C6" s="25"/>
       <c r="D6" s="25"/>
@@ -8990,23 +9579,24 @@
       <c r="BU6" s="25"/>
       <c r="BV6" s="25"/>
     </row>
-    <row r="7" spans="1:74" s="14" customFormat="1" ht="12"/>
-    <row r="8" spans="1:74" s="15" customFormat="1" ht="12"/>
+    <row r="7" s="14" customFormat="1" ht="12"/>
+    <row r="8" s="15" customFormat="1" ht="12"/>
   </sheetData>
-  <phoneticPr fontId="21" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" activeCellId="1" sqref="B10 D18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D18" sqref="B10 D18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="9" style="15" customWidth="1"/>
     <col min="2" max="2" width="15.625" style="15" customWidth="1"/>
@@ -9016,15 +9606,15 @@
     <col min="6" max="16384" width="9" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="12" customHeight="1">
+    <row r="1" customHeight="1" spans="1:2">
       <c r="A1" s="27" t="s">
         <v>164</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="37" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="12" customHeight="1">
+    <row r="4" customHeight="1" spans="1:2">
       <c r="A4" s="27" t="s">
         <v>166</v>
       </c>
@@ -9032,7 +9622,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="14.25">
+    <row r="5" ht="14.25" spans="1:2">
       <c r="A5" s="27" t="s">
         <v>166</v>
       </c>
@@ -9040,14 +9630,14 @@
         <v>168</v>
       </c>
     </row>
-    <row r="7" spans="1:5" customFormat="1" ht="13.5">
+    <row r="7" customFormat="1" ht="13.5" spans="1:5">
       <c r="A7" s="15"/>
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
     </row>
-    <row r="9" spans="1:5" ht="12" customHeight="1">
+    <row r="9" customHeight="1" spans="1:4">
       <c r="A9" s="27"/>
       <c r="B9" s="28" t="s">
         <v>176</v>
@@ -9059,49 +9649,50 @@
         <v>178</v>
       </c>
     </row>
-    <row r="10" spans="1:5" ht="12" customHeight="1">
+    <row r="10" customHeight="1" spans="1:4">
       <c r="A10" s="27" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B10" s="36" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C10" s="30" t="s">
         <v>171</v>
       </c>
       <c r="D10" s="31" t="s">
-        <v>180</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="12" customHeight="1">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="13" customHeight="1" spans="1:2">
       <c r="A13" s="27" t="s">
         <v>166</v>
       </c>
       <c r="B13" s="15" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="21" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A2:BV8"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="J36" sqref="J36"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="7"/>
   <cols>
     <col min="1" max="1" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:74" s="13" customFormat="1" ht="12.75" customHeight="1">
+    <row r="2" s="13" customFormat="1" ht="12.75" customHeight="1" spans="1:2">
       <c r="A2" s="16" t="s">
         <v>11</v>
       </c>
@@ -9109,7 +9700,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:74" s="13" customFormat="1">
+    <row r="3" s="13" customFormat="1" spans="2:71">
       <c r="B3" s="17" t="s">
         <v>13</v>
       </c>
@@ -9183,7 +9774,7 @@
       <c r="BR3" s="18"/>
       <c r="BS3" s="18"/>
     </row>
-    <row r="4" spans="1:74" s="13" customFormat="1">
+    <row r="4" s="13" customFormat="1" spans="2:74">
       <c r="B4" s="19" t="s">
         <v>14</v>
       </c>
@@ -9404,7 +9995,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:74" s="13" customFormat="1" ht="16.5" customHeight="1">
+    <row r="5" s="13" customFormat="1" ht="16.5" customHeight="1" spans="1:74">
       <c r="A5" s="21"/>
       <c r="B5" s="22" t="s">
         <v>169</v>
@@ -9626,7 +10217,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:74">
+    <row r="6" spans="2:74">
       <c r="B6" s="25"/>
       <c r="C6" s="25"/>
       <c r="D6" s="25"/>
@@ -9701,16 +10292,17 @@
       <c r="BU6" s="25"/>
       <c r="BV6" s="25"/>
     </row>
-    <row r="7" spans="1:74" s="14" customFormat="1" ht="12"/>
-    <row r="8" spans="1:74" s="15" customFormat="1" ht="12"/>
+    <row r="7" s="14" customFormat="1" ht="12"/>
+    <row r="8" s="15" customFormat="1" ht="12"/>
   </sheetData>
-  <phoneticPr fontId="21" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A3:S50"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
@@ -9726,8 +10318,8 @@
     <col min="6" max="16384" width="9" style="15"/>
   </cols>
   <sheetData>
-    <row r="3" spans="1:19" customFormat="1" ht="14.25">
-      <c r="A3" s="37" t="s">
+    <row r="3" customFormat="1" ht="14.25" spans="1:8">
+      <c r="A3" s="32" t="s">
         <v>0</v>
       </c>
       <c r="B3" s="14" t="s">
@@ -9740,8 +10332,8 @@
       <c r="G3" s="15"/>
       <c r="H3" s="15"/>
     </row>
-    <row r="4" spans="1:19" customFormat="1" ht="14.25">
-      <c r="A4" s="37" t="s">
+    <row r="4" customFormat="1" ht="14.25" spans="1:8">
+      <c r="A4" s="32" t="s">
         <v>0</v>
       </c>
       <c r="B4" s="14" t="s">
@@ -9754,8 +10346,8 @@
       <c r="G4" s="15"/>
       <c r="H4" s="15"/>
     </row>
-    <row r="5" spans="1:19" customFormat="1" ht="14.25">
-      <c r="A5" s="37" t="s">
+    <row r="5" customFormat="1" ht="14.25" spans="1:8">
+      <c r="A5" s="32" t="s">
         <v>0</v>
       </c>
       <c r="B5" s="14" t="s">
@@ -9767,8 +10359,8 @@
       <c r="G5" s="15"/>
       <c r="H5" s="15"/>
     </row>
-    <row r="6" spans="1:19" customFormat="1" ht="14.25">
-      <c r="A6" s="37" t="s">
+    <row r="6" customFormat="1" ht="14.25" spans="1:8">
+      <c r="A6" s="32" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="14" t="s">
@@ -9781,7 +10373,7 @@
       <c r="G6" s="15"/>
       <c r="H6" s="15"/>
     </row>
-    <row r="7" spans="1:19" ht="14.25">
+    <row r="7" ht="14.25" spans="1:2">
       <c r="A7" s="32" t="s">
         <v>0</v>
       </c>
@@ -9789,7 +10381,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="14.25">
+    <row r="8" ht="14.25" spans="1:7">
       <c r="A8" s="32"/>
       <c r="B8" s="14" t="s">
         <v>6</v>
@@ -9800,7 +10392,7 @@
       <c r="F8" s="14"/>
       <c r="G8" s="14"/>
     </row>
-    <row r="9" spans="1:19" ht="14.25">
+    <row r="9" ht="14.25" spans="1:7">
       <c r="A9" s="32" t="s">
         <v>0</v>
       </c>
@@ -9813,7 +10405,7 @@
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
     </row>
-    <row r="10" spans="1:19" ht="14.25">
+    <row r="10" ht="14.25" spans="1:7">
       <c r="A10" s="32" t="s">
         <v>0</v>
       </c>
@@ -9826,7 +10418,7 @@
       <c r="F10" s="14"/>
       <c r="G10" s="14"/>
     </row>
-    <row r="11" spans="1:19" ht="14.25">
+    <row r="11" ht="14.25" spans="1:7">
       <c r="A11" s="32" t="s">
         <v>0</v>
       </c>
@@ -9839,7 +10431,7 @@
       <c r="F11" s="14"/>
       <c r="G11" s="14"/>
     </row>
-    <row r="12" spans="1:19" ht="14.25">
+    <row r="12" ht="14.25" spans="1:7">
       <c r="A12" s="32" t="s">
         <v>0</v>
       </c>
@@ -9852,7 +10444,7 @@
       <c r="F12" s="14"/>
       <c r="G12" s="14"/>
     </row>
-    <row r="13" spans="1:19">
+    <row r="13" spans="1:7">
       <c r="A13" s="14"/>
       <c r="B13" s="14"/>
       <c r="C13" s="14"/>
@@ -9861,7 +10453,7 @@
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
     </row>
-    <row r="14" spans="1:19" s="14" customFormat="1" ht="14.25">
+    <row r="14" s="14" customFormat="1" ht="14.25" spans="1:2">
       <c r="A14" s="32" t="s">
         <v>11</v>
       </c>
@@ -9869,7 +10461,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="15" spans="1:19" s="14" customFormat="1">
+    <row r="15" s="14" customFormat="1" spans="2:19">
       <c r="B15" s="33" t="s">
         <v>106</v>
       </c>
@@ -9925,7 +10517,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="16" spans="1:19" s="14" customFormat="1">
+    <row r="16" s="14" customFormat="1" spans="2:19">
       <c r="B16" s="20" t="s">
         <v>108</v>
       </c>
@@ -9981,7 +10573,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="17" spans="1:19" s="14" customFormat="1">
+    <row r="17" s="14" customFormat="1" spans="2:19">
       <c r="B17" s="23" t="s">
         <v>102</v>
       </c>
@@ -10037,7 +10629,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="18" spans="1:19" s="14" customFormat="1">
+    <row r="18" s="14" customFormat="1" spans="2:19">
       <c r="B18" s="23" t="s">
         <v>99</v>
       </c>
@@ -10093,7 +10685,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="19" spans="1:19" s="14" customFormat="1">
+    <row r="19" s="14" customFormat="1" spans="2:19">
       <c r="B19" s="23" t="s">
         <v>126</v>
       </c>
@@ -10149,7 +10741,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="20" spans="1:19" s="14" customFormat="1">
+    <row r="20" s="14" customFormat="1" spans="2:19">
       <c r="B20" s="23" t="s">
         <v>129</v>
       </c>
@@ -10205,7 +10797,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="21" spans="1:19" s="14" customFormat="1">
+    <row r="21" s="14" customFormat="1" spans="2:19">
       <c r="B21" s="23" t="s">
         <v>132</v>
       </c>
@@ -10261,7 +10853,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="1:19" s="14" customFormat="1">
+    <row r="22" s="14" customFormat="1" spans="2:19">
       <c r="B22" s="23" t="s">
         <v>104</v>
       </c>
@@ -10317,7 +10909,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:19" s="14" customFormat="1">
+    <row r="23" s="14" customFormat="1" spans="2:19">
       <c r="B23" s="23" t="s">
         <v>137</v>
       </c>
@@ -10373,8 +10965,8 @@
         <v>89</v>
       </c>
     </row>
-    <row r="24" spans="1:19" s="14" customFormat="1"/>
-    <row r="26" spans="1:19" ht="14.25">
+    <row r="24" s="14" customFormat="1"/>
+    <row r="26" ht="14.25" spans="1:7">
       <c r="A26" s="32" t="s">
         <v>11</v>
       </c>
@@ -10387,7 +10979,7 @@
       <c r="F26" s="14"/>
       <c r="G26" s="14"/>
     </row>
-    <row r="27" spans="1:19">
+    <row r="27" spans="2:7">
       <c r="B27" s="33" t="s">
         <v>141</v>
       </c>
@@ -10407,7 +10999,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="1:19">
+    <row r="28" spans="1:7">
       <c r="A28" s="14"/>
       <c r="B28" s="20" t="s">
         <v>108</v>
@@ -10428,7 +11020,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="29" spans="1:19">
+    <row r="29" spans="1:7">
       <c r="A29" s="14"/>
       <c r="B29" s="23" t="s">
         <v>102</v>
@@ -10449,7 +11041,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="32" spans="1:19" ht="14.25">
+    <row r="32" ht="14.25" spans="1:10">
       <c r="A32" s="32" t="s">
         <v>11</v>
       </c>
@@ -10465,7 +11057,7 @@
       <c r="I32" s="14"/>
       <c r="J32" s="14"/>
     </row>
-    <row r="33" spans="1:13">
+    <row r="33" spans="2:10">
       <c r="B33" s="33" t="s">
         <v>144</v>
       </c>
@@ -10494,7 +11086,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="34" spans="1:13">
+    <row r="34" spans="1:10">
       <c r="A34" s="14"/>
       <c r="B34" s="20" t="s">
         <v>108</v>
@@ -10524,7 +11116,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="35" spans="1:13">
+    <row r="35" spans="1:10">
       <c r="A35" s="14"/>
       <c r="B35" s="23" t="s">
         <v>102</v>
@@ -10554,7 +11146,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="36" spans="1:13">
+    <row r="36" spans="1:10">
       <c r="A36" s="14"/>
       <c r="B36" s="23" t="s">
         <v>99</v>
@@ -10584,7 +11176,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="37" spans="1:13">
+    <row r="37" spans="1:10">
       <c r="A37" s="14"/>
       <c r="B37" s="23" t="s">
         <v>126</v>
@@ -10614,7 +11206,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="38" spans="1:13">
+    <row r="38" spans="1:10">
       <c r="A38" s="14"/>
       <c r="B38" s="23" t="s">
         <v>129</v>
@@ -10644,7 +11236,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="39" spans="1:13">
+    <row r="39" spans="1:10">
       <c r="A39" s="14"/>
       <c r="B39" s="23" t="s">
         <v>132</v>
@@ -10674,7 +11266,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="40" spans="1:13">
+    <row r="40" spans="1:10">
       <c r="A40" s="14"/>
       <c r="B40" s="23" t="s">
         <v>104</v>
@@ -10704,7 +11296,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="41" spans="1:13">
+    <row r="41" spans="1:10">
       <c r="A41" s="14"/>
       <c r="B41" s="23" t="s">
         <v>137</v>
@@ -10734,7 +11326,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="44" spans="1:13" s="14" customFormat="1" ht="14.25">
+    <row r="44" s="14" customFormat="1" ht="14.25" spans="1:2">
       <c r="A44" s="32" t="s">
         <v>11</v>
       </c>
@@ -10742,7 +11334,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="45" spans="1:13" s="14" customFormat="1">
+    <row r="45" s="14" customFormat="1" spans="2:13">
       <c r="B45" s="33" t="s">
         <v>150</v>
       </c>
@@ -10780,7 +11372,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="46" spans="1:13" s="14" customFormat="1">
+    <row r="46" s="14" customFormat="1" spans="2:13">
       <c r="B46" s="20" t="s">
         <v>108</v>
       </c>
@@ -10818,7 +11410,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="47" spans="1:13" s="14" customFormat="1">
+    <row r="47" s="14" customFormat="1" spans="2:13">
       <c r="B47" s="23" t="s">
         <v>102</v>
       </c>
@@ -10856,7 +11448,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="48" spans="1:13" s="14" customFormat="1">
+    <row r="48" s="14" customFormat="1" spans="2:13">
       <c r="B48" s="23" t="s">
         <v>99</v>
       </c>
@@ -10894,7 +11486,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="49" spans="2:13" s="14" customFormat="1">
+    <row r="49" s="14" customFormat="1" spans="2:13">
       <c r="B49" s="23" t="s">
         <v>126</v>
       </c>
@@ -10932,23 +11524,24 @@
         <v>89</v>
       </c>
     </row>
-    <row r="50" spans="2:13" s="14" customFormat="1"/>
+    <row r="50" s="14" customFormat="1"/>
   </sheetData>
-  <phoneticPr fontId="21" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:D22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="9" style="15" customWidth="1"/>
     <col min="2" max="2" width="15.625" style="15" customWidth="1"/>
@@ -10958,23 +11551,23 @@
     <col min="6" max="16384" width="9" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="12" customHeight="1">
+    <row r="1" customHeight="1" spans="1:2">
       <c r="A1" s="27" t="s">
         <v>164</v>
       </c>
-      <c r="B1" s="38" t="s">
-        <v>182</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="12" customHeight="1">
+      <c r="B1" s="37" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="3" customHeight="1" spans="1:2">
       <c r="A3" s="27" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B3" s="15" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" ht="12" customHeight="1">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="4" customHeight="1" spans="1:4">
       <c r="A4" s="27"/>
       <c r="B4" s="28" t="s">
         <v>176</v>
@@ -10986,9 +11579,9 @@
         <v>178</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="12" customHeight="1">
+    <row r="5" customHeight="1" spans="1:4">
       <c r="A5" s="27" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B5" s="29" t="s">
         <v>18</v>
@@ -11000,9 +11593,9 @@
         <v>186</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="12" customHeight="1">
+    <row r="6" customHeight="1" spans="1:4">
       <c r="A6" s="27" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B6" s="36" t="s">
         <v>19</v>
@@ -11014,9 +11607,9 @@
         <v>187</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="12" customHeight="1">
+    <row r="7" customHeight="1" spans="1:4">
       <c r="A7" s="27" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B7" s="36" t="s">
         <v>20</v>
@@ -11026,9 +11619,9 @@
         <v>188</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="12" customHeight="1">
+    <row r="8" customHeight="1" spans="1:4">
       <c r="A8" s="27" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B8" s="36" t="s">
         <v>81</v>
@@ -11040,9 +11633,9 @@
         <v>189</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="12" customHeight="1">
+    <row r="9" customHeight="1" spans="1:4">
       <c r="A9" s="27" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B9" s="36" t="s">
         <v>21</v>
@@ -11054,9 +11647,9 @@
         <v>190</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="12" customHeight="1">
+    <row r="10" customHeight="1" spans="1:4">
       <c r="A10" s="27" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B10" s="36" t="s">
         <v>23</v>
@@ -11068,9 +11661,9 @@
         <v>191</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="12" customHeight="1">
+    <row r="11" customHeight="1" spans="1:4">
       <c r="A11" s="27" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B11" s="36" t="s">
         <v>25</v>
@@ -11082,9 +11675,9 @@
         <v>192</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="12" customHeight="1">
+    <row r="12" customHeight="1" spans="1:4">
       <c r="A12" s="27" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B12" s="36" t="s">
         <v>26</v>
@@ -11096,9 +11689,9 @@
         <v>193</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="12" customHeight="1">
+    <row r="13" customHeight="1" spans="1:4">
       <c r="A13" s="27" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B13" s="36" t="s">
         <v>27</v>
@@ -11110,9 +11703,9 @@
         <v>194</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="12" customHeight="1">
+    <row r="14" customHeight="1" spans="1:4">
       <c r="A14" s="27" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B14" s="36" t="s">
         <v>195</v>
@@ -11124,9 +11717,9 @@
         <v>197</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="12" customHeight="1">
+    <row r="15" customHeight="1" spans="1:4">
       <c r="A15" s="27" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B15" s="36" t="s">
         <v>80</v>
@@ -11138,9 +11731,9 @@
         <v>198</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="12" customHeight="1">
+    <row r="16" customHeight="1" spans="1:4">
       <c r="A16" s="27" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B16" s="36" t="s">
         <v>31</v>
@@ -11152,9 +11745,9 @@
         <v>199</v>
       </c>
     </row>
-    <row r="17" spans="1:3" ht="12" customHeight="1">
+    <row r="17" customHeight="1" spans="1:3">
       <c r="A17" s="27" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B17" s="15" t="s">
         <v>32</v>
@@ -11163,7 +11756,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="22" spans="1:3" ht="12" customHeight="1">
+    <row r="22" customHeight="1" spans="1:2">
       <c r="A22" s="27" t="s">
         <v>166</v>
       </c>
@@ -11172,18 +11765,19 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="21" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A2:BV45"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:XFD6"/>
+      <selection activeCell="A2" sqref="$A2:$XFD6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5"/>
@@ -11191,7 +11785,7 @@
     <col min="1" max="1" width="9" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:74" s="13" customFormat="1" ht="12.75" customHeight="1">
+    <row r="2" s="13" customFormat="1" ht="12.75" customHeight="1" spans="1:2">
       <c r="A2" s="16" t="s">
         <v>11</v>
       </c>
@@ -11199,7 +11793,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:74" s="13" customFormat="1">
+    <row r="3" s="13" customFormat="1" spans="2:71">
       <c r="B3" s="17" t="s">
         <v>13</v>
       </c>
@@ -11273,7 +11867,7 @@
       <c r="BR3" s="18"/>
       <c r="BS3" s="18"/>
     </row>
-    <row r="4" spans="1:74" s="13" customFormat="1">
+    <row r="4" s="13" customFormat="1" spans="2:74">
       <c r="B4" s="19" t="s">
         <v>14</v>
       </c>
@@ -11494,7 +12088,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="5" spans="1:74" s="13" customFormat="1" ht="16.5" customHeight="1">
+    <row r="5" s="13" customFormat="1" ht="16.5" customHeight="1" spans="1:74">
       <c r="A5" s="21"/>
       <c r="B5" s="22" t="s">
         <v>87</v>
@@ -11716,7 +12310,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="6" spans="1:74">
+    <row r="6" spans="2:74">
       <c r="B6" s="25"/>
       <c r="C6" s="25"/>
       <c r="D6" s="25"/>
@@ -11791,7 +12385,7 @@
       <c r="BU6" s="25"/>
       <c r="BV6" s="25"/>
     </row>
-    <row r="8" spans="1:74" s="14" customFormat="1" ht="14.25">
+    <row r="8" s="14" customFormat="1" ht="14.25" spans="1:2">
       <c r="A8" s="32" t="s">
         <v>11</v>
       </c>
@@ -11799,7 +12393,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="9" spans="1:74" s="14" customFormat="1" ht="12">
+    <row r="9" s="14" customFormat="1" ht="12" spans="2:19">
       <c r="B9" s="33" t="s">
         <v>201</v>
       </c>
@@ -11855,7 +12449,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="10" spans="1:74" s="14" customFormat="1" ht="12">
+    <row r="10" s="14" customFormat="1" ht="12" spans="2:19">
       <c r="B10" s="20" t="s">
         <v>108</v>
       </c>
@@ -11911,7 +12505,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="11" spans="1:74" s="14" customFormat="1" ht="12">
+    <row r="11" s="14" customFormat="1" ht="12" spans="2:19">
       <c r="B11" s="23" t="s">
         <v>102</v>
       </c>
@@ -11967,7 +12561,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:74" s="14" customFormat="1" ht="12">
+    <row r="12" s="14" customFormat="1" ht="12" spans="2:19">
       <c r="B12" s="23" t="s">
         <v>99</v>
       </c>
@@ -12023,7 +12617,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="13" spans="1:74" s="14" customFormat="1" ht="12">
+    <row r="13" s="14" customFormat="1" ht="12" spans="2:19">
       <c r="B13" s="23" t="s">
         <v>126</v>
       </c>
@@ -12079,7 +12673,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="14" spans="1:74" s="14" customFormat="1" ht="12">
+    <row r="14" s="14" customFormat="1" ht="12" spans="2:19">
       <c r="B14" s="23" t="s">
         <v>129</v>
       </c>
@@ -12135,7 +12729,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:74" s="14" customFormat="1" ht="12">
+    <row r="15" s="14" customFormat="1" ht="12" spans="2:19">
       <c r="B15" s="23" t="s">
         <v>132</v>
       </c>
@@ -12191,7 +12785,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:74" s="14" customFormat="1" ht="12">
+    <row r="16" s="14" customFormat="1" ht="12" spans="2:19">
       <c r="B16" s="23" t="s">
         <v>104</v>
       </c>
@@ -12247,7 +12841,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="17" spans="1:19" s="14" customFormat="1" ht="12">
+    <row r="17" s="14" customFormat="1" ht="12" spans="2:19">
       <c r="B17" s="23" t="s">
         <v>137</v>
       </c>
@@ -12303,9 +12897,9 @@
         <v>89</v>
       </c>
     </row>
-    <row r="18" spans="1:19" s="14" customFormat="1" ht="12"/>
-    <row r="19" spans="1:19" s="15" customFormat="1" ht="12"/>
-    <row r="20" spans="1:19" s="15" customFormat="1" ht="14.25">
+    <row r="18" s="14" customFormat="1" ht="12"/>
+    <row r="19" s="15" customFormat="1" ht="12"/>
+    <row r="20" s="15" customFormat="1" ht="14.25" spans="1:7">
       <c r="A20" s="32" t="s">
         <v>11</v>
       </c>
@@ -12318,7 +12912,7 @@
       <c r="F20" s="14"/>
       <c r="G20" s="14"/>
     </row>
-    <row r="21" spans="1:19" s="15" customFormat="1" ht="12">
+    <row r="21" s="15" customFormat="1" ht="12" spans="2:7">
       <c r="B21" s="33" t="s">
         <v>204</v>
       </c>
@@ -12338,7 +12932,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="22" spans="1:19" s="15" customFormat="1" ht="12">
+    <row r="22" s="15" customFormat="1" ht="12" spans="1:7">
       <c r="A22" s="14"/>
       <c r="B22" s="20" t="s">
         <v>108</v>
@@ -12359,7 +12953,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="23" spans="1:19" s="15" customFormat="1" ht="12">
+    <row r="23" s="15" customFormat="1" ht="12" spans="1:7">
       <c r="A23" s="14"/>
       <c r="B23" s="23" t="s">
         <v>102</v>
@@ -12380,9 +12974,9 @@
         <v>142</v>
       </c>
     </row>
-    <row r="24" spans="1:19" s="15" customFormat="1" ht="12"/>
-    <row r="25" spans="1:19" s="15" customFormat="1" ht="12"/>
-    <row r="26" spans="1:19" s="15" customFormat="1" ht="14.25">
+    <row r="24" s="15" customFormat="1" ht="12"/>
+    <row r="25" s="15" customFormat="1" ht="12"/>
+    <row r="26" s="15" customFormat="1" ht="14.25" spans="1:10">
       <c r="A26" s="32" t="s">
         <v>11</v>
       </c>
@@ -12398,7 +12992,7 @@
       <c r="I26" s="14"/>
       <c r="J26" s="14"/>
     </row>
-    <row r="27" spans="1:19" s="15" customFormat="1" ht="12">
+    <row r="27" s="15" customFormat="1" ht="12" spans="2:10">
       <c r="B27" s="33" t="s">
         <v>205</v>
       </c>
@@ -12427,7 +13021,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="28" spans="1:19" s="15" customFormat="1" ht="12">
+    <row r="28" s="15" customFormat="1" ht="12" spans="1:10">
       <c r="A28" s="14"/>
       <c r="B28" s="20" t="s">
         <v>108</v>
@@ -12457,7 +13051,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="29" spans="1:19" s="15" customFormat="1" ht="12">
+    <row r="29" s="15" customFormat="1" ht="12" spans="1:10">
       <c r="A29" s="14"/>
       <c r="B29" s="23" t="s">
         <v>102</v>
@@ -12487,7 +13081,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="30" spans="1:19" s="15" customFormat="1" ht="12">
+    <row r="30" s="15" customFormat="1" ht="12" spans="1:10">
       <c r="A30" s="14"/>
       <c r="B30" s="23" t="s">
         <v>99</v>
@@ -12517,7 +13111,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="31" spans="1:19" s="15" customFormat="1" ht="12">
+    <row r="31" s="15" customFormat="1" ht="12" spans="1:10">
       <c r="A31" s="14"/>
       <c r="B31" s="23" t="s">
         <v>126</v>
@@ -12547,7 +13141,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="32" spans="1:19" s="15" customFormat="1" ht="12">
+    <row r="32" s="15" customFormat="1" ht="12" spans="1:10">
       <c r="A32" s="14"/>
       <c r="B32" s="23" t="s">
         <v>129</v>
@@ -12577,7 +13171,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="33" spans="1:13" s="15" customFormat="1" ht="12">
+    <row r="33" s="15" customFormat="1" ht="12" spans="1:10">
       <c r="A33" s="14"/>
       <c r="B33" s="23" t="s">
         <v>132</v>
@@ -12607,7 +13201,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="34" spans="1:13" s="15" customFormat="1" ht="12">
+    <row r="34" s="15" customFormat="1" ht="12" spans="1:10">
       <c r="A34" s="14"/>
       <c r="B34" s="23" t="s">
         <v>104</v>
@@ -12637,7 +13231,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="35" spans="1:13" s="15" customFormat="1" ht="12">
+    <row r="35" s="15" customFormat="1" ht="12" spans="1:10">
       <c r="A35" s="14"/>
       <c r="B35" s="23" t="s">
         <v>137</v>
@@ -12667,9 +13261,9 @@
         <v>137</v>
       </c>
     </row>
-    <row r="36" spans="1:13" s="15" customFormat="1" ht="12"/>
-    <row r="37" spans="1:13" s="15" customFormat="1" ht="12"/>
-    <row r="38" spans="1:13" s="14" customFormat="1" ht="14.25">
+    <row r="36" s="15" customFormat="1" ht="12"/>
+    <row r="37" s="15" customFormat="1" ht="12"/>
+    <row r="38" s="14" customFormat="1" ht="14.25" spans="1:2">
       <c r="A38" s="32" t="s">
         <v>11</v>
       </c>
@@ -12677,7 +13271,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="39" spans="1:13" s="14" customFormat="1" ht="12">
+    <row r="39" s="14" customFormat="1" ht="12" spans="2:13">
       <c r="B39" s="33" t="s">
         <v>207</v>
       </c>
@@ -12715,7 +13309,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="40" spans="1:13" s="14" customFormat="1" ht="12">
+    <row r="40" s="14" customFormat="1" ht="12" spans="2:13">
       <c r="B40" s="20" t="s">
         <v>108</v>
       </c>
@@ -12753,7 +13347,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="41" spans="1:13" s="14" customFormat="1" ht="12">
+    <row r="41" s="14" customFormat="1" ht="12" spans="2:13">
       <c r="B41" s="23" t="s">
         <v>102</v>
       </c>
@@ -12791,7 +13385,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="42" spans="1:13" s="14" customFormat="1" ht="12">
+    <row r="42" s="14" customFormat="1" ht="12" spans="2:13">
       <c r="B42" s="23" t="s">
         <v>99</v>
       </c>
@@ -12829,7 +13423,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="43" spans="1:13" s="14" customFormat="1" ht="12">
+    <row r="43" s="14" customFormat="1" ht="12" spans="2:13">
       <c r="B43" s="23" t="s">
         <v>126</v>
       </c>
@@ -12867,23 +13461,24 @@
         <v>89</v>
       </c>
     </row>
-    <row r="44" spans="1:13" s="14" customFormat="1" ht="12"/>
-    <row r="45" spans="1:13" s="15" customFormat="1" ht="12"/>
+    <row r="44" s="14" customFormat="1" ht="12"/>
+    <row r="45" s="15" customFormat="1" ht="12"/>
   </sheetData>
-  <phoneticPr fontId="21" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView topLeftCell="A4" workbookViewId="0">
       <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="9" style="15" customWidth="1"/>
     <col min="2" max="2" width="15.625" style="15" customWidth="1"/>
@@ -12893,15 +13488,15 @@
     <col min="6" max="16384" width="9" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="12" customHeight="1">
+    <row r="1" customHeight="1" spans="1:2">
       <c r="A1" s="27" t="s">
         <v>164</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="37" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="12" customHeight="1">
+    <row r="4" customHeight="1" spans="1:2">
       <c r="A4" s="27" t="s">
         <v>166</v>
       </c>
@@ -12909,7 +13504,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="14.25">
+    <row r="5" ht="14.25" spans="1:2">
       <c r="A5" s="27" t="s">
         <v>166</v>
       </c>
@@ -12917,14 +13512,14 @@
         <v>168</v>
       </c>
     </row>
-    <row r="7" spans="1:5" customFormat="1" ht="13.5">
+    <row r="7" customFormat="1" ht="13.5" spans="1:5">
       <c r="A7" s="15"/>
       <c r="B7" s="15"/>
       <c r="C7" s="15"/>
       <c r="D7" s="15"/>
       <c r="E7" s="15"/>
     </row>
-    <row r="9" spans="1:5" ht="14.25">
+    <row r="9" ht="14.25" spans="1:2">
       <c r="A9" s="27" t="s">
         <v>166</v>
       </c>
@@ -12932,15 +13527,15 @@
         <v>212</v>
       </c>
     </row>
-    <row r="12" spans="1:5" ht="12" customHeight="1">
+    <row r="12" customHeight="1" spans="1:2">
       <c r="A12" s="27" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="B12" s="15" t="s">
-        <v>184</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="12" customHeight="1">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="13" customHeight="1" spans="1:4">
       <c r="A13" s="27"/>
       <c r="B13" s="28" t="s">
         <v>176</v>
@@ -12952,9 +13547,9 @@
         <v>178</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="12" customHeight="1">
+    <row r="14" customHeight="1" spans="1:4">
       <c r="A14" s="27" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B14" s="29" t="s">
         <v>18</v>
@@ -12966,9 +13561,9 @@
         <v>186</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="12" customHeight="1">
+    <row r="15" customHeight="1" spans="1:4">
       <c r="A15" s="27" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B15" s="36" t="s">
         <v>19</v>
@@ -12980,9 +13575,9 @@
         <v>187</v>
       </c>
     </row>
-    <row r="16" spans="1:5" ht="12" customHeight="1">
+    <row r="16" customHeight="1" spans="1:4">
       <c r="A16" s="27" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B16" s="36" t="s">
         <v>20</v>
@@ -12992,9 +13587,9 @@
         <v>188</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="12" customHeight="1">
+    <row r="17" customHeight="1" spans="1:4">
       <c r="A17" s="27" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B17" s="36" t="s">
         <v>81</v>
@@ -13006,9 +13601,9 @@
         <v>189</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="12" customHeight="1">
+    <row r="18" customHeight="1" spans="1:4">
       <c r="A18" s="27" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B18" s="36" t="s">
         <v>21</v>
@@ -13020,9 +13615,9 @@
         <v>190</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="12" customHeight="1">
+    <row r="19" customHeight="1" spans="1:4">
       <c r="A19" s="27" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B19" s="36" t="s">
         <v>23</v>
@@ -13034,9 +13629,9 @@
         <v>191</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="12" customHeight="1">
+    <row r="20" customHeight="1" spans="1:4">
       <c r="A20" s="27" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B20" s="36" t="s">
         <v>25</v>
@@ -13048,9 +13643,9 @@
         <v>192</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="12" customHeight="1">
+    <row r="21" customHeight="1" spans="1:4">
       <c r="A21" s="27" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B21" s="36" t="s">
         <v>26</v>
@@ -13062,9 +13657,9 @@
         <v>193</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="12" customHeight="1">
+    <row r="22" customHeight="1" spans="1:4">
       <c r="A22" s="27" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B22" s="36" t="s">
         <v>27</v>
@@ -13076,9 +13671,9 @@
         <v>194</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="12" customHeight="1">
+    <row r="23" customHeight="1" spans="1:4">
       <c r="A23" s="27" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B23" s="36" t="s">
         <v>195</v>
@@ -13090,9 +13685,9 @@
         <v>197</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="12" customHeight="1">
+    <row r="24" customHeight="1" spans="1:4">
       <c r="A24" s="27" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B24" s="36" t="s">
         <v>80</v>
@@ -13104,9 +13699,9 @@
         <v>198</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="12" customHeight="1">
+    <row r="25" customHeight="1" spans="1:4">
       <c r="A25" s="27" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B25" s="36" t="s">
         <v>31</v>
@@ -13118,9 +13713,9 @@
         <v>199</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="12" customHeight="1">
+    <row r="26" customHeight="1" spans="1:3">
       <c r="A26" s="27" t="s">
-        <v>185</v>
+        <v>179</v>
       </c>
       <c r="B26" s="15" t="s">
         <v>32</v>
@@ -13129,7 +13724,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="30" spans="1:4" ht="12" customHeight="1">
+    <row r="30" customHeight="1" spans="1:2">
       <c r="A30" s="27" t="s">
         <v>166</v>
       </c>
@@ -13137,7 +13732,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="14.25">
+    <row r="31" ht="14.25" spans="1:2">
       <c r="A31" s="27" t="s">
         <v>166</v>
       </c>
@@ -13146,8 +13741,8 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="21" type="noConversion"/>
-  <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>